<commit_message>
Added textFilePopulator logic for reference sequences
</commit_message>
<xml_diff>
--- a/tabular/hiv-reference-data.xlsx
+++ b/tabular/hiv-reference-data.xlsx
@@ -21,9 +21,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="120">
   <si>
-    <t xml:space="preserve">Subtype </t>
-  </si>
-  <si>
     <t>B</t>
   </si>
   <si>
@@ -84,9 +81,6 @@
     <t>Year</t>
   </si>
   <si>
-    <t>Country of Origin</t>
-  </si>
-  <si>
     <t>Reference</t>
   </si>
   <si>
@@ -379,6 +373,12 @@
   </si>
   <si>
     <t>Isolate</t>
+  </si>
+  <si>
+    <t>Subtype</t>
+  </si>
+  <si>
+    <t>Country</t>
   </si>
 </sst>
 </file>
@@ -1162,7 +1162,7 @@
   <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1177,44 +1177,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="11" customFormat="1">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="B1" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="B1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="F1" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="G1" s="18" t="s">
         <v>20</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" s="22" t="s">
-        <v>117</v>
-      </c>
-      <c r="G1" s="18" t="s">
-        <v>22</v>
       </c>
       <c r="H1" s="9"/>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>1</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>2</v>
       </c>
       <c r="D2" s="15">
         <v>1983</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F2" s="23">
         <v>9181</v>
@@ -1226,19 +1226,19 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="16" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="16" t="s">
         <v>1</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>2</v>
       </c>
       <c r="D3" s="15">
         <v>1983</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F3" s="24">
         <v>9719</v>
@@ -1250,19 +1250,19 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F4" s="25">
         <v>9000</v>
@@ -1274,19 +1274,19 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F5" s="25">
         <v>14825</v>
@@ -1298,43 +1298,43 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D6" s="12">
         <v>2014</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F6" s="25">
         <v>9709</v>
       </c>
       <c r="G6" s="17" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D7" s="9">
         <v>1990</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F7" s="26">
         <v>8996</v>
@@ -1346,10 +1346,10 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8" s="6">
         <v>671</v>
@@ -1358,7 +1358,7 @@
         <v>2000</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F8" s="26">
         <v>9359</v>
@@ -1370,10 +1370,10 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9" s="6">
         <v>1058</v>
@@ -1382,7 +1382,7 @@
         <v>1998</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F9" s="26">
         <v>8834</v>
@@ -1394,19 +1394,19 @@
     </row>
     <row r="10" spans="1:8" ht="18" customHeight="1">
       <c r="A10" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D10" s="8">
         <v>1992</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F10" s="28">
         <v>8999</v>
@@ -1418,19 +1418,19 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D11" s="8">
         <v>1994</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F11" s="28">
         <v>9160</v>
@@ -1442,19 +1442,19 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D12" s="9">
         <v>1994</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F12" s="26">
         <v>8813</v>
@@ -1466,19 +1466,19 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D13" s="9">
         <v>1998</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F13" s="26">
         <v>8807</v>
@@ -1490,19 +1490,19 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D14" s="9">
         <v>1997</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F14" s="26">
         <v>8972</v>
@@ -1514,19 +1514,19 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D15" s="9">
         <v>1994</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F15" s="26">
         <v>9060</v>
@@ -1538,19 +1538,19 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D16" s="9">
         <v>1986</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F16" s="26">
         <v>9031</v>
@@ -1562,19 +1562,19 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D17" s="9">
         <v>1992</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F17" s="26">
         <v>8959</v>
@@ -1586,19 +1586,19 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D18" s="8">
         <v>1995</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F18" s="26">
         <v>9002</v>
@@ -1610,19 +1610,19 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D19" s="8">
         <v>2004</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F19" s="26">
         <v>9011</v>
@@ -1634,19 +1634,19 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D20" s="8">
         <v>1983</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F20" s="26">
         <v>9176</v>
@@ -1658,19 +1658,19 @@
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D21" s="8">
         <v>1994</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F21" s="26">
         <v>8952</v>
@@ -1682,19 +1682,19 @@
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D22" s="8">
         <v>2001</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F22" s="26">
         <v>8379</v>
@@ -1706,19 +1706,19 @@
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D23" s="8">
         <v>2001</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F23" s="26">
         <v>8775</v>
@@ -1730,19 +1730,19 @@
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D24" s="8">
         <v>1993</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F24" s="26">
         <v>8968</v>
@@ -1754,19 +1754,19 @@
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D25" s="8">
         <v>1993</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F25" s="26">
         <v>8903</v>
@@ -1778,19 +1778,19 @@
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D26" s="8">
         <v>1993</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F26" s="26">
         <v>8925</v>
@@ -1802,19 +1802,19 @@
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D27" s="8">
         <v>1996</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F27" s="26">
         <v>8614</v>
@@ -1826,19 +1826,19 @@
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D28" s="8">
         <v>1995</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F28" s="26">
         <v>8555</v>
@@ -1850,19 +1850,19 @@
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D29" s="8">
         <v>1995</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F29" s="26">
         <v>8589</v>
@@ -1874,19 +1874,19 @@
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D30" s="8">
         <v>2002</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F30" s="26">
         <v>8349</v>
@@ -1898,19 +1898,19 @@
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D31" s="8">
         <v>1997</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F31" s="26">
         <v>8782</v>
@@ -1922,19 +1922,19 @@
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D32" s="8">
         <v>1993</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F32" s="26">
         <v>9074</v>
@@ -1946,19 +1946,19 @@
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D33" s="8">
         <v>1993</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F33" s="26">
         <v>9048</v>
@@ -1970,19 +1970,19 @@
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D34" s="8">
         <v>1996</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F34" s="26">
         <v>9707</v>
@@ -1994,19 +1994,19 @@
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D35" s="8">
         <v>1992</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F35" s="26">
         <v>8987</v>
@@ -2018,19 +2018,19 @@
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D36" s="8">
         <v>1990</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F36" s="26">
         <v>8953</v>
@@ -2042,19 +2042,19 @@
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D37" s="8">
         <v>1994</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F37" s="26">
         <v>9056</v>
@@ -2066,19 +2066,19 @@
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D38" s="8">
         <v>1993</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F38" s="26">
         <v>8955</v>
@@ -2090,19 +2090,19 @@
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D39" s="8">
         <v>1994</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F39" s="26">
         <v>8943</v>
@@ -2114,19 +2114,19 @@
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D40" s="8">
         <v>1993</v>
       </c>
       <c r="E40" s="8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F40" s="26">
         <v>8953</v>
@@ -2138,19 +2138,19 @@
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D41" s="8">
         <v>1997</v>
       </c>
       <c r="E41" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F41" s="26">
         <v>8600</v>
@@ -2162,19 +2162,19 @@
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D42" s="8">
         <v>1996</v>
       </c>
       <c r="E42" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F42" s="26">
         <v>8604</v>

</xml_diff>

<commit_message>
Added reference sequence data for common CRFs
</commit_message>
<xml_diff>
--- a/tabular/hiv-reference-data.xlsx
+++ b/tabular/hiv-reference-data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4660" yWindow="0" windowWidth="22380" windowHeight="28360" tabRatio="500"/>
+    <workbookView xWindow="16540" yWindow="4660" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="141">
   <si>
     <t>B</t>
   </si>
@@ -379,6 +379,69 @@
   </si>
   <si>
     <t>Country</t>
+  </si>
+  <si>
+    <t>01_AE</t>
+  </si>
+  <si>
+    <t>CM240</t>
+  </si>
+  <si>
+    <t>U54771</t>
+  </si>
+  <si>
+    <t>02_AG</t>
+  </si>
+  <si>
+    <t>IBNG</t>
+  </si>
+  <si>
+    <t>L39106</t>
+  </si>
+  <si>
+    <t>06_AGJK</t>
+  </si>
+  <si>
+    <t>BFP90</t>
+  </si>
+  <si>
+    <t>AF064699</t>
+  </si>
+  <si>
+    <t>Australia (Burkina Faso)</t>
+  </si>
+  <si>
+    <t>07_BC</t>
+  </si>
+  <si>
+    <t>CN54</t>
+  </si>
+  <si>
+    <t>AX149771</t>
+  </si>
+  <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>08_BC</t>
+  </si>
+  <si>
+    <t>GX-6F</t>
+  </si>
+  <si>
+    <t>AY008715</t>
+  </si>
+  <si>
+    <t>12_BF</t>
+  </si>
+  <si>
+    <t>ARMA159</t>
+  </si>
+  <si>
+    <t>AF385936</t>
+  </si>
+  <si>
+    <t>Argentina</t>
   </si>
 </sst>
 </file>
@@ -499,7 +562,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="129">
+  <cellStyleXfs count="159">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -629,8 +692,38 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -656,9 +749,6 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -679,29 +769,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="129">
+  <cellStyles count="159">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -829,7 +912,37 @@
     <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="127" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1159,96 +1272,92 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H42"/>
+  <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="28" customWidth="1"/>
+    <col min="1" max="1" width="13.5" customWidth="1"/>
     <col min="3" max="3" width="28.83203125" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" style="11" customWidth="1"/>
     <col min="5" max="5" width="16.5" customWidth="1"/>
-    <col min="6" max="6" width="20.83203125" style="27" customWidth="1"/>
-    <col min="7" max="7" width="25.33203125" style="21" customWidth="1"/>
-    <col min="8" max="8" width="17.83203125" customWidth="1"/>
+    <col min="6" max="6" width="20.83203125" style="30" customWidth="1"/>
+    <col min="7" max="7" width="25.33203125" style="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="11" customFormat="1">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:7" s="11" customFormat="1">
+      <c r="A1" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="17" t="s">
         <v>117</v>
       </c>
       <c r="D1" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="23" t="s">
         <v>119</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="F1" s="23" t="s">
         <v>115</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="9"/>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="14" t="s">
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="13" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="15">
+      <c r="D2" s="14">
         <v>1983</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="F2" s="23">
+      <c r="F2" s="28">
         <v>9181</v>
       </c>
-      <c r="G2" s="19">
+      <c r="G2" s="18">
         <v>9362478</v>
       </c>
-      <c r="H2" s="1"/>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="16" t="s">
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="15" t="s">
         <v>42</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="15">
+      <c r="D3" s="14">
         <v>1983</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="F3" s="24">
+      <c r="F3" s="29">
         <v>9719</v>
       </c>
-      <c r="G3" s="20">
+      <c r="G3" s="19">
         <v>2578615</v>
       </c>
-      <c r="H3" s="1"/>
-    </row>
-    <row r="4" spans="1:8">
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="5" t="s">
         <v>7</v>
       </c>
@@ -1261,18 +1370,17 @@
       <c r="D4" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="25" t="s">
         <v>111</v>
       </c>
       <c r="F4" s="25">
         <v>9000</v>
       </c>
-      <c r="G4" s="17">
+      <c r="G4" s="16">
         <v>7483282</v>
       </c>
-      <c r="H4" s="1"/>
-    </row>
-    <row r="5" spans="1:8">
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="5" t="s">
         <v>6</v>
       </c>
@@ -1285,18 +1393,17 @@
       <c r="D5" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="25" t="s">
         <v>111</v>
       </c>
       <c r="F5" s="25">
         <v>14825</v>
       </c>
-      <c r="G5" s="17">
+      <c r="G5" s="16">
         <v>3016298</v>
       </c>
-      <c r="H5" s="1"/>
-    </row>
-    <row r="6" spans="1:8">
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
@@ -1309,18 +1416,17 @@
       <c r="D6" s="12">
         <v>2014</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="25" t="s">
         <v>49</v>
       </c>
       <c r="F6" s="25">
         <v>9709</v>
       </c>
-      <c r="G6" s="17" t="s">
+      <c r="G6" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="H6" s="1"/>
-    </row>
-    <row r="7" spans="1:8">
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" s="3" t="s">
         <v>43</v>
       </c>
@@ -1333,7 +1439,7 @@
       <c r="D7" s="9">
         <v>1990</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="26" t="s">
         <v>47</v>
       </c>
       <c r="F7" s="26">
@@ -1342,9 +1448,8 @@
       <c r="G7" s="6">
         <v>12487805</v>
       </c>
-      <c r="H7" s="1"/>
-    </row>
-    <row r="8" spans="1:8">
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="3" t="s">
         <v>44</v>
       </c>
@@ -1357,7 +1462,7 @@
       <c r="D8" s="9">
         <v>2000</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="26" t="s">
         <v>48</v>
       </c>
       <c r="F8" s="26">
@@ -1366,9 +1471,8 @@
       <c r="G8" s="6">
         <v>14610167</v>
       </c>
-      <c r="H8" s="1"/>
-    </row>
-    <row r="9" spans="1:8">
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" s="3" t="s">
         <v>45</v>
       </c>
@@ -1381,7 +1485,7 @@
       <c r="D9" s="9">
         <v>1998</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="26" t="s">
         <v>49</v>
       </c>
       <c r="F9" s="26">
@@ -1390,9 +1494,8 @@
       <c r="G9" s="6">
         <v>16103205</v>
       </c>
-      <c r="H9" s="1"/>
-    </row>
-    <row r="10" spans="1:8" ht="18" customHeight="1">
+    </row>
+    <row r="10" spans="1:7" ht="18" customHeight="1">
       <c r="A10" s="3" t="s">
         <v>22</v>
       </c>
@@ -1405,18 +1508,17 @@
       <c r="D10" s="8">
         <v>1992</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="F10" s="28">
+      <c r="F10" s="27">
         <v>8999</v>
       </c>
       <c r="G10" s="6">
         <v>8794346</v>
       </c>
-      <c r="H10" s="1"/>
-    </row>
-    <row r="11" spans="1:8">
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" s="3" t="s">
         <v>34</v>
       </c>
@@ -1429,18 +1531,17 @@
       <c r="D11" s="8">
         <v>1994</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E11" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="F11" s="28">
+      <c r="F11" s="27">
         <v>9160</v>
       </c>
-      <c r="G11" s="21">
+      <c r="G11" s="20">
         <v>10364271</v>
       </c>
-      <c r="H11" s="1"/>
-    </row>
-    <row r="12" spans="1:8">
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" s="1" t="s">
         <v>36</v>
       </c>
@@ -1453,7 +1554,7 @@
       <c r="D12" s="9">
         <v>1994</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="E12" s="26" t="s">
         <v>107</v>
       </c>
       <c r="F12" s="26">
@@ -1462,9 +1563,8 @@
       <c r="G12" s="6">
         <v>10513639</v>
       </c>
-      <c r="H12" s="1"/>
-    </row>
-    <row r="13" spans="1:8">
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" s="1" t="s">
         <v>37</v>
       </c>
@@ -1477,7 +1577,7 @@
       <c r="D13" s="9">
         <v>1998</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="26" t="s">
         <v>21</v>
       </c>
       <c r="F13" s="26">
@@ -1486,9 +1586,8 @@
       <c r="G13" s="6">
         <v>12487816</v>
       </c>
-      <c r="H13" s="1"/>
-    </row>
-    <row r="14" spans="1:8">
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" s="1" t="s">
         <v>38</v>
       </c>
@@ -1501,7 +1600,7 @@
       <c r="D14" s="9">
         <v>1997</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="E14" s="26" t="s">
         <v>40</v>
       </c>
       <c r="F14" s="26">
@@ -1510,9 +1609,8 @@
       <c r="G14" s="6">
         <v>11429108</v>
       </c>
-      <c r="H14" s="1"/>
-    </row>
-    <row r="15" spans="1:8">
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" s="1" t="s">
         <v>39</v>
       </c>
@@ -1525,7 +1623,7 @@
       <c r="D15" s="9">
         <v>1994</v>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="E15" s="26" t="s">
         <v>41</v>
       </c>
       <c r="F15" s="26">
@@ -1534,9 +1632,8 @@
       <c r="G15" s="6">
         <v>11429108</v>
       </c>
-      <c r="H15" s="1"/>
-    </row>
-    <row r="16" spans="1:8">
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" s="3" t="s">
         <v>50</v>
       </c>
@@ -1549,7 +1646,7 @@
       <c r="D16" s="9">
         <v>1986</v>
       </c>
-      <c r="E16" s="9" t="s">
+      <c r="E16" s="26" t="s">
         <v>54</v>
       </c>
       <c r="F16" s="26">
@@ -1558,9 +1655,8 @@
       <c r="G16" s="6">
         <v>8891112</v>
       </c>
-      <c r="H16" s="1"/>
-    </row>
-    <row r="17" spans="1:8">
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" s="3" t="s">
         <v>51</v>
       </c>
@@ -1573,7 +1669,7 @@
       <c r="D17" s="9">
         <v>1992</v>
       </c>
-      <c r="E17" s="9" t="s">
+      <c r="E17" s="26" t="s">
         <v>55</v>
       </c>
       <c r="F17" s="26">
@@ -1582,9 +1678,8 @@
       <c r="G17" s="6">
         <v>8627686</v>
       </c>
-      <c r="H17" s="1"/>
-    </row>
-    <row r="18" spans="1:8">
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" s="3" t="s">
         <v>52</v>
       </c>
@@ -1597,7 +1692,7 @@
       <c r="D18" s="8">
         <v>1995</v>
       </c>
-      <c r="E18" s="8" t="s">
+      <c r="E18" s="27" t="s">
         <v>56</v>
       </c>
       <c r="F18" s="26">
@@ -1606,9 +1701,8 @@
       <c r="G18" s="6">
         <v>9847317</v>
       </c>
-      <c r="H18" s="1"/>
-    </row>
-    <row r="19" spans="1:8">
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" s="3" t="s">
         <v>53</v>
       </c>
@@ -1621,7 +1715,7 @@
       <c r="D19" s="8">
         <v>2004</v>
       </c>
-      <c r="E19" s="8" t="s">
+      <c r="E19" s="27" t="s">
         <v>57</v>
       </c>
       <c r="F19" s="26">
@@ -1630,9 +1724,8 @@
       <c r="G19" s="6">
         <v>15592417</v>
       </c>
-      <c r="H19" s="1"/>
-    </row>
-    <row r="20" spans="1:8">
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" s="3" t="s">
         <v>58</v>
       </c>
@@ -1645,7 +1738,7 @@
       <c r="D20" s="8">
         <v>1983</v>
       </c>
-      <c r="E20" s="8" t="s">
+      <c r="E20" s="27" t="s">
         <v>40</v>
       </c>
       <c r="F20" s="26">
@@ -1654,9 +1747,8 @@
       <c r="G20" s="6">
         <v>2424612</v>
       </c>
-      <c r="H20" s="1"/>
-    </row>
-    <row r="21" spans="1:8">
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" s="3" t="s">
         <v>59</v>
       </c>
@@ -1669,7 +1761,7 @@
       <c r="D21" s="8">
         <v>1994</v>
       </c>
-      <c r="E21" s="8" t="s">
+      <c r="E21" s="27" t="s">
         <v>21</v>
       </c>
       <c r="F21" s="26">
@@ -1678,9 +1770,8 @@
       <c r="G21" s="6">
         <v>9621027</v>
       </c>
-      <c r="H21" s="1"/>
-    </row>
-    <row r="22" spans="1:8">
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22" s="3" t="s">
         <v>60</v>
       </c>
@@ -1693,7 +1784,7 @@
       <c r="D22" s="8">
         <v>2001</v>
       </c>
-      <c r="E22" s="8" t="s">
+      <c r="E22" s="27" t="s">
         <v>62</v>
       </c>
       <c r="F22" s="26">
@@ -1702,9 +1793,8 @@
       <c r="G22" s="6">
         <v>15186527</v>
       </c>
-      <c r="H22" s="1"/>
-    </row>
-    <row r="23" spans="1:8">
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23" s="3" t="s">
         <v>61</v>
       </c>
@@ -1717,7 +1807,7 @@
       <c r="D23" s="8">
         <v>2001</v>
       </c>
-      <c r="E23" s="8" t="s">
+      <c r="E23" s="27" t="s">
         <v>63</v>
       </c>
       <c r="F23" s="26">
@@ -1726,9 +1816,8 @@
       <c r="G23" s="6">
         <v>15320994</v>
       </c>
-      <c r="H23" s="1"/>
-    </row>
-    <row r="24" spans="1:8">
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24" s="3" t="s">
         <v>68</v>
       </c>
@@ -1741,7 +1830,7 @@
       <c r="D24" s="8">
         <v>1993</v>
       </c>
-      <c r="E24" s="8" t="s">
+      <c r="E24" s="27" t="s">
         <v>55</v>
       </c>
       <c r="F24" s="26">
@@ -1750,9 +1839,8 @@
       <c r="G24" s="6">
         <v>9621027</v>
       </c>
-      <c r="H24" s="1"/>
-    </row>
-    <row r="25" spans="1:8">
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25" s="3" t="s">
         <v>69</v>
       </c>
@@ -1765,7 +1853,7 @@
       <c r="D25" s="8">
         <v>1993</v>
       </c>
-      <c r="E25" s="8" t="s">
+      <c r="E25" s="27" t="s">
         <v>40</v>
       </c>
       <c r="F25" s="26">
@@ -1774,9 +1862,8 @@
       <c r="G25" s="6">
         <v>10725202</v>
       </c>
-      <c r="H25" s="1"/>
-    </row>
-    <row r="26" spans="1:8">
+    </row>
+    <row r="26" spans="1:7">
       <c r="A26" s="3" t="s">
         <v>70</v>
       </c>
@@ -1789,7 +1876,7 @@
       <c r="D26" s="8">
         <v>1993</v>
       </c>
-      <c r="E26" s="8" t="s">
+      <c r="E26" s="27" t="s">
         <v>72</v>
       </c>
       <c r="F26" s="26">
@@ -1798,9 +1885,8 @@
       <c r="G26" s="6">
         <v>10725203</v>
       </c>
-      <c r="H26" s="1"/>
-    </row>
-    <row r="27" spans="1:8">
+    </row>
+    <row r="27" spans="1:7">
       <c r="A27" s="3" t="s">
         <v>71</v>
       </c>
@@ -1813,7 +1899,7 @@
       <c r="D27" s="8">
         <v>1996</v>
       </c>
-      <c r="E27" s="8" t="s">
+      <c r="E27" s="27" t="s">
         <v>46</v>
       </c>
       <c r="F27" s="26">
@@ -1822,9 +1908,8 @@
       <c r="G27" s="6">
         <v>10659053</v>
       </c>
-      <c r="H27" s="1"/>
-    </row>
-    <row r="28" spans="1:8">
+    </row>
+    <row r="28" spans="1:7">
       <c r="A28" s="3" t="s">
         <v>74</v>
       </c>
@@ -1837,7 +1922,7 @@
       <c r="D28" s="8">
         <v>1995</v>
       </c>
-      <c r="E28" s="8" t="s">
+      <c r="E28" s="27" t="s">
         <v>62</v>
       </c>
       <c r="F28" s="26">
@@ -1846,9 +1931,8 @@
       <c r="G28" s="6">
         <v>10659054</v>
       </c>
-      <c r="H28" s="1"/>
-    </row>
-    <row r="29" spans="1:8">
+    </row>
+    <row r="29" spans="1:7">
       <c r="A29" s="3" t="s">
         <v>77</v>
       </c>
@@ -1861,7 +1945,7 @@
       <c r="D29" s="8">
         <v>1995</v>
       </c>
-      <c r="E29" s="8" t="s">
+      <c r="E29" s="27" t="s">
         <v>62</v>
       </c>
       <c r="F29" s="26">
@@ -1870,9 +1954,8 @@
       <c r="G29" s="6">
         <v>10659055</v>
       </c>
-      <c r="H29" s="1"/>
-    </row>
-    <row r="30" spans="1:8">
+    </row>
+    <row r="30" spans="1:7">
       <c r="A30" s="3" t="s">
         <v>78</v>
       </c>
@@ -1885,7 +1968,7 @@
       <c r="D30" s="8">
         <v>2002</v>
       </c>
-      <c r="E30" s="8" t="s">
+      <c r="E30" s="27" t="s">
         <v>62</v>
       </c>
       <c r="F30" s="26">
@@ -1894,9 +1977,8 @@
       <c r="G30" s="6">
         <v>15186527</v>
       </c>
-      <c r="H30" s="1"/>
-    </row>
-    <row r="31" spans="1:8">
+    </row>
+    <row r="31" spans="1:7">
       <c r="A31" s="3" t="s">
         <v>80</v>
       </c>
@@ -1909,7 +1991,7 @@
       <c r="D31" s="8">
         <v>1997</v>
       </c>
-      <c r="E31" s="8" t="s">
+      <c r="E31" s="27" t="s">
         <v>62</v>
       </c>
       <c r="F31" s="26">
@@ -1918,9 +2000,8 @@
       <c r="G31" s="6">
         <v>11448170</v>
       </c>
-      <c r="H31" s="1"/>
-    </row>
-    <row r="32" spans="1:8">
+    </row>
+    <row r="32" spans="1:7">
       <c r="A32" s="3" t="s">
         <v>82</v>
       </c>
@@ -1933,7 +2014,7 @@
       <c r="D32" s="8">
         <v>1993</v>
       </c>
-      <c r="E32" s="8" t="s">
+      <c r="E32" s="27" t="s">
         <v>86</v>
       </c>
       <c r="F32" s="26">
@@ -1942,9 +2023,8 @@
       <c r="G32" s="6">
         <v>9683568</v>
       </c>
-      <c r="H32" s="1"/>
-    </row>
-    <row r="33" spans="1:8">
+    </row>
+    <row r="33" spans="1:7">
       <c r="A33" s="3" t="s">
         <v>84</v>
       </c>
@@ -1957,7 +2037,7 @@
       <c r="D33" s="8">
         <v>1993</v>
       </c>
-      <c r="E33" s="8" t="s">
+      <c r="E33" s="27" t="s">
         <v>85</v>
       </c>
       <c r="F33" s="26">
@@ -1966,9 +2046,8 @@
       <c r="G33" s="6">
         <v>9683569</v>
       </c>
-      <c r="H33" s="1"/>
-    </row>
-    <row r="34" spans="1:8">
+    </row>
+    <row r="34" spans="1:7">
       <c r="A34" s="3" t="s">
         <v>88</v>
       </c>
@@ -1981,7 +2060,7 @@
       <c r="D34" s="8">
         <v>1996</v>
       </c>
-      <c r="E34" s="8" t="s">
+      <c r="E34" s="27" t="s">
         <v>40</v>
       </c>
       <c r="F34" s="26">
@@ -1990,9 +2069,8 @@
       <c r="G34" s="6">
         <v>10221535</v>
       </c>
-      <c r="H34" s="1"/>
-    </row>
-    <row r="35" spans="1:8">
+    </row>
+    <row r="35" spans="1:7">
       <c r="A35" s="3" t="s">
         <v>90</v>
       </c>
@@ -2005,7 +2083,7 @@
       <c r="D35" s="8">
         <v>1992</v>
       </c>
-      <c r="E35" s="8" t="s">
+      <c r="E35" s="27" t="s">
         <v>91</v>
       </c>
       <c r="F35" s="26">
@@ -2014,9 +2092,8 @@
       <c r="G35" s="6">
         <v>9621027</v>
       </c>
-      <c r="H35" s="1"/>
-    </row>
-    <row r="36" spans="1:8">
+    </row>
+    <row r="36" spans="1:7">
       <c r="A36" s="3" t="s">
         <v>92</v>
       </c>
@@ -2029,7 +2106,7 @@
       <c r="D36" s="8">
         <v>1990</v>
       </c>
-      <c r="E36" s="8" t="s">
+      <c r="E36" s="27" t="s">
         <v>93</v>
       </c>
       <c r="F36" s="26">
@@ -2038,9 +2115,8 @@
       <c r="G36" s="6">
         <v>9621028</v>
       </c>
-      <c r="H36" s="1"/>
-    </row>
-    <row r="37" spans="1:8">
+    </row>
+    <row r="37" spans="1:7">
       <c r="A37" s="3" t="s">
         <v>95</v>
       </c>
@@ -2053,7 +2129,7 @@
       <c r="D37" s="8">
         <v>1994</v>
       </c>
-      <c r="E37" s="8" t="s">
+      <c r="E37" s="27" t="s">
         <v>113</v>
       </c>
       <c r="F37" s="26">
@@ -2062,9 +2138,8 @@
       <c r="G37" s="6">
         <v>10983640</v>
       </c>
-      <c r="H37" s="1"/>
-    </row>
-    <row r="38" spans="1:8">
+    </row>
+    <row r="38" spans="1:7">
       <c r="A38" s="3" t="s">
         <v>97</v>
       </c>
@@ -2077,7 +2152,7 @@
       <c r="D38" s="8">
         <v>1993</v>
       </c>
-      <c r="E38" s="8" t="s">
+      <c r="E38" s="27" t="s">
         <v>113</v>
       </c>
       <c r="F38" s="26">
@@ -2086,9 +2161,8 @@
       <c r="G38" s="6">
         <v>10983641</v>
       </c>
-      <c r="H38" s="1"/>
-    </row>
-    <row r="39" spans="1:8">
+    </row>
+    <row r="39" spans="1:7">
       <c r="A39" s="3" t="s">
         <v>99</v>
       </c>
@@ -2101,7 +2175,7 @@
       <c r="D39" s="8">
         <v>1994</v>
       </c>
-      <c r="E39" s="8" t="s">
+      <c r="E39" s="27" t="s">
         <v>86</v>
       </c>
       <c r="F39" s="26">
@@ -2110,9 +2184,8 @@
       <c r="G39" s="6">
         <v>10052760</v>
       </c>
-      <c r="H39" s="1"/>
-    </row>
-    <row r="40" spans="1:8">
+    </row>
+    <row r="40" spans="1:7">
       <c r="A40" s="3" t="s">
         <v>101</v>
       </c>
@@ -2125,7 +2198,7 @@
       <c r="D40" s="8">
         <v>1993</v>
       </c>
-      <c r="E40" s="8" t="s">
+      <c r="E40" s="27" t="s">
         <v>86</v>
       </c>
       <c r="F40" s="26">
@@ -2134,9 +2207,8 @@
       <c r="G40" s="6">
         <v>10052761</v>
       </c>
-      <c r="H40" s="1"/>
-    </row>
-    <row r="41" spans="1:8">
+    </row>
+    <row r="41" spans="1:7">
       <c r="A41" s="3" t="s">
         <v>103</v>
       </c>
@@ -2149,7 +2221,7 @@
       <c r="D41" s="8">
         <v>1997</v>
       </c>
-      <c r="E41" s="8" t="s">
+      <c r="E41" s="27" t="s">
         <v>40</v>
       </c>
       <c r="F41" s="26">
@@ -2158,9 +2230,8 @@
       <c r="G41" s="6">
         <v>10659053</v>
       </c>
-      <c r="H41" s="1"/>
-    </row>
-    <row r="42" spans="1:8">
+    </row>
+    <row r="42" spans="1:7">
       <c r="A42" s="3" t="s">
         <v>105</v>
       </c>
@@ -2173,7 +2244,7 @@
       <c r="D42" s="8">
         <v>1996</v>
       </c>
-      <c r="E42" s="8" t="s">
+      <c r="E42" s="27" t="s">
         <v>62</v>
       </c>
       <c r="F42" s="26">
@@ -2182,7 +2253,142 @@
       <c r="G42" s="6">
         <v>10659054</v>
       </c>
-      <c r="H42" s="1"/>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="B43" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="C43" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="D43" s="8">
+        <v>1990</v>
+      </c>
+      <c r="E43" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="F43" s="27">
+        <v>9203</v>
+      </c>
+      <c r="G43" s="21">
+        <v>8709215</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="B44" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="C44" s="21" t="s">
+        <v>124</v>
+      </c>
+      <c r="D44" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="E44" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="F44" s="27">
+        <v>9201</v>
+      </c>
+      <c r="G44" s="21">
+        <v>7888238</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="B45" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="C45" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="D45" s="8">
+        <v>1996</v>
+      </c>
+      <c r="E45" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="F45" s="27">
+        <v>9775</v>
+      </c>
+      <c r="G45" s="21">
+        <v>9824329</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="B46" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="C46" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="D46" s="8">
+        <v>1997</v>
+      </c>
+      <c r="E46" s="27" t="s">
+        <v>133</v>
+      </c>
+      <c r="F46" s="27">
+        <v>9078</v>
+      </c>
+      <c r="G46" s="21"/>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="B47" s="22" t="s">
+        <v>134</v>
+      </c>
+      <c r="C47" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="D47" s="8">
+        <v>1997</v>
+      </c>
+      <c r="E47" s="27" t="s">
+        <v>133</v>
+      </c>
+      <c r="F47" s="27">
+        <v>8802</v>
+      </c>
+      <c r="G47" s="21">
+        <v>11070028</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="B48" s="22" t="s">
+        <v>137</v>
+      </c>
+      <c r="C48" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="D48" s="8">
+        <v>1991</v>
+      </c>
+      <c r="E48" s="27" t="s">
+        <v>140</v>
+      </c>
+      <c r="F48" s="27">
+        <v>9704</v>
+      </c>
+      <c r="G48" s="21">
+        <v>11600844</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Merged modules from HIV-CONVAR
</commit_message>
<xml_diff>
--- a/tabular/hiv-reference-data.xlsx
+++ b/tabular/hiv-reference-data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="20260" yWindow="100" windowWidth="25460" windowHeight="25220" tabRatio="500"/>
+    <workbookView xWindow="9640" yWindow="340" windowWidth="25460" windowHeight="25220" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="edited down" sheetId="1" r:id="rId1"/>
@@ -2932,7 +2932,7 @@
   <dimension ref="A1:S162"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="A1:K162"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Introduced subtype A into convar build
</commit_message>
<xml_diff>
--- a/tabular/hiv-reference-data.xlsx
+++ b/tabular/hiv-reference-data.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2553" uniqueCount="526">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2561" uniqueCount="527">
   <si>
     <t>Accession</t>
   </si>
@@ -1599,6 +1599,9 @@
   </si>
   <si>
     <t>Ferret</t>
+  </si>
+  <si>
+    <t>AM279354</t>
   </si>
 </sst>
 </file>
@@ -1763,7 +1766,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="370">
+  <cellStyleXfs count="376">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2105,6 +2108,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2213,7 +2222,7 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="370">
+  <cellStyles count="376">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2414,6 +2423,9 @@
     <cellStyle name="Followed Hyperlink" xfId="365" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="367" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="369" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="371" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="373" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="375" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2583,6 +2595,9 @@
     <cellStyle name="Hyperlink" xfId="364" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="366" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="368" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="370" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="372" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="374" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
@@ -2929,10 +2944,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S162"/>
+  <dimension ref="A1:S163"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3383,8 +3398,8 @@
       <c r="S15" s="9"/>
     </row>
     <row r="16" spans="1:19">
-      <c r="A16" s="16" t="s">
-        <v>27</v>
+      <c r="A16" s="15" t="s">
+        <v>526</v>
       </c>
       <c r="B16" s="15" t="s">
         <v>446</v>
@@ -3395,17 +3410,13 @@
       <c r="D16" s="15" t="s">
         <v>374</v>
       </c>
-      <c r="E16" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="F16" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="G16" s="15">
-        <v>1992</v>
-      </c>
+      <c r="E16" s="15" t="s">
+        <v>454</v>
+      </c>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
       <c r="H16" s="16" t="s">
-        <v>30</v>
+        <v>66</v>
       </c>
       <c r="I16" s="16" t="s">
         <v>435</v>
@@ -3414,7 +3425,7 @@
         <v>316</v>
       </c>
       <c r="K16" s="15">
-        <v>8794346</v>
+        <v>16817969</v>
       </c>
       <c r="L16" s="9"/>
       <c r="M16" s="9"/>
@@ -3427,7 +3438,7 @@
     </row>
     <row r="17" spans="1:19">
       <c r="A17" s="16" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B17" s="15" t="s">
         <v>446</v>
@@ -3442,13 +3453,13 @@
         <v>28</v>
       </c>
       <c r="F17" s="16" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G17" s="15">
-        <v>1994</v>
+        <v>1992</v>
       </c>
       <c r="H17" s="16" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="I17" s="16" t="s">
         <v>435</v>
@@ -3457,20 +3468,20 @@
         <v>316</v>
       </c>
       <c r="K17" s="15">
-        <v>10364271</v>
+        <v>8794346</v>
       </c>
       <c r="L17" s="9"/>
       <c r="M17" s="9"/>
-      <c r="N17" s="1"/>
-      <c r="O17" s="10"/>
-      <c r="P17" s="1"/>
-      <c r="Q17" s="1"/>
+      <c r="N17" s="9"/>
+      <c r="O17" s="9"/>
+      <c r="P17" s="9"/>
+      <c r="Q17" s="9"/>
       <c r="R17" s="9"/>
       <c r="S17" s="9"/>
     </row>
     <row r="18" spans="1:19">
       <c r="A18" s="16" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B18" s="15" t="s">
         <v>446</v>
@@ -3485,13 +3496,13 @@
         <v>28</v>
       </c>
       <c r="F18" s="16" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G18" s="15">
         <v>1994</v>
       </c>
       <c r="H18" s="16" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="I18" s="16" t="s">
         <v>435</v>
@@ -3500,20 +3511,20 @@
         <v>316</v>
       </c>
       <c r="K18" s="15">
-        <v>10513639</v>
+        <v>10364271</v>
       </c>
       <c r="L18" s="9"/>
       <c r="M18" s="9"/>
-      <c r="N18" s="9"/>
-      <c r="O18" s="9"/>
-      <c r="P18" s="9"/>
-      <c r="Q18" s="9"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="10"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
       <c r="R18" s="9"/>
       <c r="S18" s="9"/>
     </row>
     <row r="19" spans="1:19">
       <c r="A19" s="16" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B19" s="15" t="s">
         <v>446</v>
@@ -3528,13 +3539,13 @@
         <v>28</v>
       </c>
       <c r="F19" s="16" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G19" s="15">
-        <v>1998</v>
+        <v>1994</v>
       </c>
       <c r="H19" s="16" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="I19" s="16" t="s">
         <v>435</v>
@@ -3543,7 +3554,7 @@
         <v>316</v>
       </c>
       <c r="K19" s="15">
-        <v>12487816</v>
+        <v>10513639</v>
       </c>
       <c r="L19" s="9"/>
       <c r="M19" s="9"/>
@@ -3556,7 +3567,7 @@
     </row>
     <row r="20" spans="1:19">
       <c r="A20" s="16" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B20" s="15" t="s">
         <v>446</v>
@@ -3568,16 +3579,16 @@
         <v>374</v>
       </c>
       <c r="E20" s="16" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="F20" s="16" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G20" s="15">
-        <v>1997</v>
+        <v>1998</v>
       </c>
       <c r="H20" s="16" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="I20" s="16" t="s">
         <v>435</v>
@@ -3586,7 +3597,7 @@
         <v>316</v>
       </c>
       <c r="K20" s="15">
-        <v>11429108</v>
+        <v>12487816</v>
       </c>
       <c r="L20" s="9"/>
       <c r="M20" s="9"/>
@@ -3599,7 +3610,7 @@
     </row>
     <row r="21" spans="1:19">
       <c r="A21" s="16" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B21" s="15" t="s">
         <v>446</v>
@@ -3614,13 +3625,13 @@
         <v>40</v>
       </c>
       <c r="F21" s="16" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G21" s="15">
-        <v>1994</v>
+        <v>1997</v>
       </c>
       <c r="H21" s="16" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="I21" s="16" t="s">
         <v>435</v>
@@ -3642,7 +3653,7 @@
     </row>
     <row r="22" spans="1:19">
       <c r="A22" s="16" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="B22" s="15" t="s">
         <v>446</v>
@@ -3654,16 +3665,16 @@
         <v>374</v>
       </c>
       <c r="E22" s="16" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="F22" s="16" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="G22" s="15">
-        <v>1983</v>
+        <v>1994</v>
       </c>
       <c r="H22" s="16" t="s">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="I22" s="16" t="s">
         <v>435</v>
@@ -3672,7 +3683,7 @@
         <v>316</v>
       </c>
       <c r="K22" s="15">
-        <v>9362478</v>
+        <v>11429108</v>
       </c>
       <c r="L22" s="9"/>
       <c r="M22" s="9"/>
@@ -3685,7 +3696,7 @@
     </row>
     <row r="23" spans="1:19">
       <c r="A23" s="16" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B23" s="15" t="s">
         <v>446</v>
@@ -3700,13 +3711,13 @@
         <v>8</v>
       </c>
       <c r="F23" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="G23" s="15" t="s">
-        <v>14</v>
+        <v>9</v>
+      </c>
+      <c r="G23" s="15">
+        <v>1983</v>
       </c>
       <c r="H23" s="16" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="I23" s="16" t="s">
         <v>435</v>
@@ -3715,7 +3726,7 @@
         <v>316</v>
       </c>
       <c r="K23" s="15">
-        <v>7483282</v>
+        <v>9362478</v>
       </c>
       <c r="L23" s="9"/>
       <c r="M23" s="9"/>
@@ -3728,7 +3739,7 @@
     </row>
     <row r="24" spans="1:19">
       <c r="A24" s="16" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B24" s="15" t="s">
         <v>446</v>
@@ -3743,7 +3754,7 @@
         <v>8</v>
       </c>
       <c r="F24" s="16" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G24" s="15" t="s">
         <v>14</v>
@@ -3758,7 +3769,7 @@
         <v>316</v>
       </c>
       <c r="K24" s="15">
-        <v>3016298</v>
+        <v>7483282</v>
       </c>
       <c r="L24" s="9"/>
       <c r="M24" s="9"/>
@@ -3771,7 +3782,7 @@
     </row>
     <row r="25" spans="1:19">
       <c r="A25" s="16" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B25" s="15" t="s">
         <v>446</v>
@@ -3786,13 +3797,13 @@
         <v>8</v>
       </c>
       <c r="F25" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="G25" s="15">
-        <v>2014</v>
+        <v>16</v>
+      </c>
+      <c r="G25" s="15" t="s">
+        <v>14</v>
       </c>
       <c r="H25" s="16" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="I25" s="16" t="s">
         <v>435</v>
@@ -3800,8 +3811,8 @@
       <c r="J25" s="16" t="s">
         <v>316</v>
       </c>
-      <c r="K25" s="15" t="s">
-        <v>20</v>
+      <c r="K25" s="15">
+        <v>3016298</v>
       </c>
       <c r="L25" s="9"/>
       <c r="M25" s="9"/>
@@ -3814,7 +3825,7 @@
     </row>
     <row r="26" spans="1:19">
       <c r="A26" s="16" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B26" s="15" t="s">
         <v>446</v>
@@ -3829,13 +3840,13 @@
         <v>8</v>
       </c>
       <c r="F26" s="16" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="G26" s="15">
-        <v>1990</v>
+        <v>2014</v>
       </c>
       <c r="H26" s="16" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="I26" s="16" t="s">
         <v>435</v>
@@ -3843,34 +3854,42 @@
       <c r="J26" s="16" t="s">
         <v>316</v>
       </c>
-      <c r="K26" s="15">
-        <v>12487805</v>
+      <c r="K26" s="15" t="s">
+        <v>20</v>
       </c>
       <c r="L26" s="9"/>
       <c r="M26" s="9"/>
-      <c r="N26" s="1"/>
-      <c r="O26" s="10"/>
-      <c r="P26" s="1"/>
-      <c r="Q26" s="1"/>
+      <c r="N26" s="9"/>
+      <c r="O26" s="9"/>
+      <c r="P26" s="9"/>
+      <c r="Q26" s="9"/>
       <c r="R26" s="9"/>
       <c r="S26" s="9"/>
     </row>
     <row r="27" spans="1:19">
-      <c r="A27" t="s">
-        <v>177</v>
-      </c>
-      <c r="B27" s="18" t="s">
+      <c r="A27" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B27" s="15" t="s">
         <v>446</v>
       </c>
       <c r="C27" s="16" t="s">
         <v>348</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>377</v>
-      </c>
-      <c r="F27"/>
+        <v>374</v>
+      </c>
+      <c r="E27" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="F27" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="G27" s="15">
+        <v>1990</v>
+      </c>
       <c r="H27" s="16" t="s">
-        <v>66</v>
+        <v>23</v>
       </c>
       <c r="I27" s="16" t="s">
         <v>435</v>
@@ -3878,13 +3897,21 @@
       <c r="J27" s="16" t="s">
         <v>316</v>
       </c>
-      <c r="K27" s="1">
-        <v>8107220</v>
-      </c>
+      <c r="K27" s="15">
+        <v>12487805</v>
+      </c>
+      <c r="L27" s="9"/>
+      <c r="M27" s="9"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="10"/>
+      <c r="P27" s="1"/>
+      <c r="Q27" s="1"/>
+      <c r="R27" s="9"/>
+      <c r="S27" s="9"/>
     </row>
     <row r="28" spans="1:19">
       <c r="A28" t="s">
-        <v>11</v>
+        <v>177</v>
       </c>
       <c r="B28" s="18" t="s">
         <v>446</v>
@@ -3893,15 +3920,12 @@
         <v>348</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>374</v>
-      </c>
-      <c r="E28" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="F28" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="H28" s="16"/>
+        <v>377</v>
+      </c>
+      <c r="F28"/>
+      <c r="H28" s="16" t="s">
+        <v>66</v>
+      </c>
       <c r="I28" s="16" t="s">
         <v>435</v>
       </c>
@@ -3909,14 +3933,14 @@
         <v>316</v>
       </c>
       <c r="K28" s="1">
-        <v>2578615</v>
+        <v>8107220</v>
       </c>
     </row>
     <row r="29" spans="1:19">
-      <c r="A29" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="B29" s="15" t="s">
+      <c r="A29" t="s">
+        <v>11</v>
+      </c>
+      <c r="B29" s="18" t="s">
         <v>446</v>
       </c>
       <c r="C29" s="16" t="s">
@@ -3928,36 +3952,23 @@
       <c r="E29" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="F29" s="15">
-        <v>671</v>
-      </c>
-      <c r="G29" s="15">
-        <v>2000</v>
-      </c>
-      <c r="H29" s="16" t="s">
-        <v>25</v>
-      </c>
+      <c r="F29" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="H29" s="16"/>
       <c r="I29" s="16" t="s">
         <v>435</v>
       </c>
       <c r="J29" s="16" t="s">
         <v>316</v>
       </c>
-      <c r="K29" s="15">
-        <v>14610167</v>
-      </c>
-      <c r="L29" s="9"/>
-      <c r="M29" s="9"/>
-      <c r="N29" s="9"/>
-      <c r="O29" s="9"/>
-      <c r="P29" s="9"/>
-      <c r="Q29" s="9"/>
-      <c r="R29" s="9"/>
-      <c r="S29" s="9"/>
+      <c r="K29" s="1">
+        <v>2578615</v>
+      </c>
     </row>
     <row r="30" spans="1:19">
       <c r="A30" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B30" s="15" t="s">
         <v>446</v>
@@ -3972,13 +3983,13 @@
         <v>8</v>
       </c>
       <c r="F30" s="15">
-        <v>1058</v>
+        <v>671</v>
       </c>
       <c r="G30" s="15">
-        <v>1998</v>
+        <v>2000</v>
       </c>
       <c r="H30" s="16" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="I30" s="16" t="s">
         <v>435</v>
@@ -3987,7 +3998,7 @@
         <v>316</v>
       </c>
       <c r="K30" s="15">
-        <v>16103205</v>
+        <v>14610167</v>
       </c>
       <c r="L30" s="9"/>
       <c r="M30" s="9"/>
@@ -4000,7 +4011,7 @@
     </row>
     <row r="31" spans="1:19">
       <c r="A31" s="16" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="B31" s="15" t="s">
         <v>446</v>
@@ -4012,16 +4023,16 @@
         <v>374</v>
       </c>
       <c r="E31" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="F31" s="16" t="s">
-        <v>48</v>
+        <v>8</v>
+      </c>
+      <c r="F31" s="15">
+        <v>1058</v>
       </c>
       <c r="G31" s="15">
-        <v>1986</v>
+        <v>1998</v>
       </c>
       <c r="H31" s="16" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="I31" s="16" t="s">
         <v>435</v>
@@ -4030,12 +4041,20 @@
         <v>316</v>
       </c>
       <c r="K31" s="15">
-        <v>8891112</v>
-      </c>
+        <v>16103205</v>
+      </c>
+      <c r="L31" s="9"/>
+      <c r="M31" s="9"/>
+      <c r="N31" s="9"/>
+      <c r="O31" s="9"/>
+      <c r="P31" s="9"/>
+      <c r="Q31" s="9"/>
+      <c r="R31" s="9"/>
+      <c r="S31" s="9"/>
     </row>
     <row r="32" spans="1:19">
       <c r="A32" s="16" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B32" s="15" t="s">
         <v>446</v>
@@ -4050,13 +4069,13 @@
         <v>47</v>
       </c>
       <c r="F32" s="16" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="G32" s="15">
-        <v>1992</v>
+        <v>1986</v>
       </c>
       <c r="H32" s="16" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="I32" s="16" t="s">
         <v>435</v>
@@ -4065,12 +4084,12 @@
         <v>316</v>
       </c>
       <c r="K32" s="15">
-        <v>8627686</v>
+        <v>8891112</v>
       </c>
     </row>
     <row r="33" spans="1:11">
       <c r="A33" s="16" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B33" s="15" t="s">
         <v>446</v>
@@ -4085,13 +4104,13 @@
         <v>47</v>
       </c>
       <c r="F33" s="16" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="G33" s="15">
-        <v>1995</v>
+        <v>1992</v>
       </c>
       <c r="H33" s="16" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I33" s="16" t="s">
         <v>435</v>
@@ -4100,12 +4119,12 @@
         <v>316</v>
       </c>
       <c r="K33" s="15">
-        <v>9847317</v>
+        <v>8627686</v>
       </c>
     </row>
     <row r="34" spans="1:11">
       <c r="A34" s="16" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B34" s="15" t="s">
         <v>446</v>
@@ -4120,13 +4139,13 @@
         <v>47</v>
       </c>
       <c r="F34" s="16" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G34" s="15">
-        <v>2004</v>
+        <v>1995</v>
       </c>
       <c r="H34" s="16" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="I34" s="16" t="s">
         <v>435</v>
@@ -4135,12 +4154,12 @@
         <v>316</v>
       </c>
       <c r="K34" s="15">
-        <v>15592417</v>
+        <v>9847317</v>
       </c>
     </row>
     <row r="35" spans="1:11">
-      <c r="A35" s="15" t="s">
-        <v>133</v>
+      <c r="A35" s="16" t="s">
+        <v>56</v>
       </c>
       <c r="B35" s="15" t="s">
         <v>446</v>
@@ -4151,17 +4170,17 @@
       <c r="D35" s="15" t="s">
         <v>374</v>
       </c>
-      <c r="E35" s="15" t="s">
+      <c r="E35" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="F35" s="15" t="s">
-        <v>134</v>
+      <c r="F35" s="16" t="s">
+        <v>57</v>
       </c>
       <c r="G35" s="15">
-        <v>1997</v>
+        <v>2004</v>
       </c>
       <c r="H35" s="16" t="s">
-        <v>132</v>
+        <v>58</v>
       </c>
       <c r="I35" s="16" t="s">
         <v>435</v>
@@ -4170,12 +4189,12 @@
         <v>316</v>
       </c>
       <c r="K35" s="15">
-        <v>11070028</v>
+        <v>15592417</v>
       </c>
     </row>
     <row r="36" spans="1:11">
-      <c r="A36" s="16" t="s">
-        <v>59</v>
+      <c r="A36" s="15" t="s">
+        <v>133</v>
       </c>
       <c r="B36" s="15" t="s">
         <v>446</v>
@@ -4186,17 +4205,17 @@
       <c r="D36" s="15" t="s">
         <v>374</v>
       </c>
-      <c r="E36" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="F36" s="16" t="s">
-        <v>61</v>
+      <c r="E36" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="F36" s="15" t="s">
+        <v>134</v>
       </c>
       <c r="G36" s="15">
-        <v>1983</v>
+        <v>1997</v>
       </c>
       <c r="H36" s="16" t="s">
-        <v>42</v>
+        <v>132</v>
       </c>
       <c r="I36" s="16" t="s">
         <v>435</v>
@@ -4205,12 +4224,12 @@
         <v>316</v>
       </c>
       <c r="K36" s="15">
-        <v>2424612</v>
+        <v>11070028</v>
       </c>
     </row>
     <row r="37" spans="1:11">
       <c r="A37" s="16" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B37" s="15" t="s">
         <v>446</v>
@@ -4225,13 +4244,13 @@
         <v>60</v>
       </c>
       <c r="F37" s="16" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G37" s="15">
-        <v>1994</v>
+        <v>1983</v>
       </c>
       <c r="H37" s="16" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="I37" s="16" t="s">
         <v>435</v>
@@ -4240,12 +4259,12 @@
         <v>316</v>
       </c>
       <c r="K37" s="15">
-        <v>9621027</v>
+        <v>2424612</v>
       </c>
     </row>
     <row r="38" spans="1:11">
       <c r="A38" s="16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B38" s="15" t="s">
         <v>446</v>
@@ -4260,13 +4279,13 @@
         <v>60</v>
       </c>
       <c r="F38" s="16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G38" s="15">
-        <v>2001</v>
+        <v>1994</v>
       </c>
       <c r="H38" s="16" t="s">
-        <v>66</v>
+        <v>30</v>
       </c>
       <c r="I38" s="16" t="s">
         <v>435</v>
@@ -4275,12 +4294,12 @@
         <v>316</v>
       </c>
       <c r="K38" s="15">
-        <v>15186527</v>
+        <v>9621027</v>
       </c>
     </row>
     <row r="39" spans="1:11">
       <c r="A39" s="16" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B39" s="15" t="s">
         <v>446</v>
@@ -4295,13 +4314,13 @@
         <v>60</v>
       </c>
       <c r="F39" s="16" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="G39" s="15">
         <v>2001</v>
       </c>
       <c r="H39" s="16" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="I39" s="16" t="s">
         <v>435</v>
@@ -4310,12 +4329,12 @@
         <v>316</v>
       </c>
       <c r="K39" s="15">
-        <v>15320994</v>
+        <v>15186527</v>
       </c>
     </row>
     <row r="40" spans="1:11">
       <c r="A40" s="16" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B40" s="15" t="s">
         <v>446</v>
@@ -4327,16 +4346,16 @@
         <v>374</v>
       </c>
       <c r="E40" s="16" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="F40" s="16" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="G40" s="15">
-        <v>1993</v>
+        <v>2001</v>
       </c>
       <c r="H40" s="16" t="s">
-        <v>52</v>
+        <v>69</v>
       </c>
       <c r="I40" s="16" t="s">
         <v>435</v>
@@ -4345,12 +4364,12 @@
         <v>316</v>
       </c>
       <c r="K40" s="15">
-        <v>9621027</v>
+        <v>15320994</v>
       </c>
     </row>
     <row r="41" spans="1:11">
       <c r="A41" s="16" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B41" s="15" t="s">
         <v>446</v>
@@ -4365,13 +4384,13 @@
         <v>71</v>
       </c>
       <c r="F41" s="16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G41" s="15">
         <v>1993</v>
       </c>
       <c r="H41" s="16" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="I41" s="16" t="s">
         <v>435</v>
@@ -4380,12 +4399,12 @@
         <v>316</v>
       </c>
       <c r="K41" s="15">
-        <v>10725202</v>
+        <v>9621027</v>
       </c>
     </row>
     <row r="42" spans="1:11">
       <c r="A42" s="16" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B42" s="15" t="s">
         <v>446</v>
@@ -4400,13 +4419,13 @@
         <v>71</v>
       </c>
       <c r="F42" s="16" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G42" s="15">
         <v>1993</v>
       </c>
       <c r="H42" s="16" t="s">
-        <v>77</v>
+        <v>42</v>
       </c>
       <c r="I42" s="16" t="s">
         <v>435</v>
@@ -4415,12 +4434,12 @@
         <v>316</v>
       </c>
       <c r="K42" s="15">
-        <v>10725203</v>
+        <v>10725202</v>
       </c>
     </row>
     <row r="43" spans="1:11">
       <c r="A43" s="16" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B43" s="15" t="s">
         <v>446</v>
@@ -4435,13 +4454,13 @@
         <v>71</v>
       </c>
       <c r="F43" s="16" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="G43" s="15">
-        <v>1996</v>
+        <v>1993</v>
       </c>
       <c r="H43" s="16" t="s">
-        <v>10</v>
+        <v>77</v>
       </c>
       <c r="I43" s="16" t="s">
         <v>435</v>
@@ -4450,12 +4469,12 @@
         <v>316</v>
       </c>
       <c r="K43" s="15">
-        <v>10659053</v>
+        <v>10725203</v>
       </c>
     </row>
     <row r="44" spans="1:11">
       <c r="A44" s="16" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B44" s="15" t="s">
         <v>446</v>
@@ -4470,13 +4489,13 @@
         <v>71</v>
       </c>
       <c r="F44" s="16" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G44" s="15">
-        <v>1995</v>
+        <v>1996</v>
       </c>
       <c r="H44" s="16" t="s">
-        <v>66</v>
+        <v>10</v>
       </c>
       <c r="I44" s="16" t="s">
         <v>435</v>
@@ -4485,12 +4504,12 @@
         <v>316</v>
       </c>
       <c r="K44" s="15">
-        <v>10659054</v>
+        <v>10659053</v>
       </c>
     </row>
     <row r="45" spans="1:11">
       <c r="A45" s="16" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B45" s="15" t="s">
         <v>446</v>
@@ -4505,7 +4524,7 @@
         <v>71</v>
       </c>
       <c r="F45" s="16" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G45" s="15">
         <v>1995</v>
@@ -4520,12 +4539,12 @@
         <v>316</v>
       </c>
       <c r="K45" s="15">
-        <v>10659055</v>
+        <v>10659054</v>
       </c>
     </row>
     <row r="46" spans="1:11">
       <c r="A46" s="16" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B46" s="15" t="s">
         <v>446</v>
@@ -4540,10 +4559,10 @@
         <v>71</v>
       </c>
       <c r="F46" s="16" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G46" s="15">
-        <v>2002</v>
+        <v>1995</v>
       </c>
       <c r="H46" s="16" t="s">
         <v>66</v>
@@ -4555,12 +4574,12 @@
         <v>316</v>
       </c>
       <c r="K46" s="15">
-        <v>15186527</v>
+        <v>10659055</v>
       </c>
     </row>
     <row r="47" spans="1:11">
       <c r="A47" s="16" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B47" s="15" t="s">
         <v>446</v>
@@ -4575,10 +4594,10 @@
         <v>71</v>
       </c>
       <c r="F47" s="16" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G47" s="15">
-        <v>1997</v>
+        <v>2002</v>
       </c>
       <c r="H47" s="16" t="s">
         <v>66</v>
@@ -4590,12 +4609,12 @@
         <v>316</v>
       </c>
       <c r="K47" s="15">
-        <v>11448170</v>
+        <v>15186527</v>
       </c>
     </row>
     <row r="48" spans="1:11">
-      <c r="A48" s="15" t="s">
-        <v>135</v>
+      <c r="A48" s="16" t="s">
+        <v>86</v>
       </c>
       <c r="B48" s="15" t="s">
         <v>446</v>
@@ -4606,17 +4625,17 @@
       <c r="D48" s="15" t="s">
         <v>374</v>
       </c>
-      <c r="E48" s="15" t="s">
+      <c r="E48" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="F48" s="15" t="s">
-        <v>136</v>
+      <c r="F48" s="16" t="s">
+        <v>87</v>
       </c>
       <c r="G48" s="15">
-        <v>1991</v>
+        <v>1997</v>
       </c>
       <c r="H48" s="16" t="s">
-        <v>137</v>
+        <v>66</v>
       </c>
       <c r="I48" s="16" t="s">
         <v>435</v>
@@ -4625,12 +4644,12 @@
         <v>316</v>
       </c>
       <c r="K48" s="15">
-        <v>11600844</v>
+        <v>11448170</v>
       </c>
     </row>
     <row r="49" spans="1:11">
-      <c r="A49" s="16" t="s">
-        <v>88</v>
+      <c r="A49" s="15" t="s">
+        <v>135</v>
       </c>
       <c r="B49" s="15" t="s">
         <v>446</v>
@@ -4641,17 +4660,17 @@
       <c r="D49" s="15" t="s">
         <v>374</v>
       </c>
-      <c r="E49" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="F49" s="16" t="s">
-        <v>90</v>
+      <c r="E49" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="F49" s="15" t="s">
+        <v>136</v>
       </c>
       <c r="G49" s="15">
-        <v>1993</v>
+        <v>1991</v>
       </c>
       <c r="H49" s="16" t="s">
-        <v>91</v>
+        <v>137</v>
       </c>
       <c r="I49" s="16" t="s">
         <v>435</v>
@@ -4660,12 +4679,12 @@
         <v>316</v>
       </c>
       <c r="K49" s="15">
-        <v>9683568</v>
+        <v>11600844</v>
       </c>
     </row>
     <row r="50" spans="1:11">
       <c r="A50" s="16" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B50" s="15" t="s">
         <v>446</v>
@@ -4680,13 +4699,13 @@
         <v>89</v>
       </c>
       <c r="F50" s="16" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="G50" s="15">
         <v>1993</v>
       </c>
       <c r="H50" s="16" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="I50" s="16" t="s">
         <v>435</v>
@@ -4695,12 +4714,12 @@
         <v>316</v>
       </c>
       <c r="K50" s="15">
-        <v>9683569</v>
+        <v>9683568</v>
       </c>
     </row>
     <row r="51" spans="1:11">
       <c r="A51" s="16" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B51" s="15" t="s">
         <v>446</v>
@@ -4715,13 +4734,13 @@
         <v>89</v>
       </c>
       <c r="F51" s="16" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G51" s="15">
-        <v>1996</v>
+        <v>1993</v>
       </c>
       <c r="H51" s="16" t="s">
-        <v>42</v>
+        <v>94</v>
       </c>
       <c r="I51" s="16" t="s">
         <v>435</v>
@@ -4730,12 +4749,12 @@
         <v>316</v>
       </c>
       <c r="K51" s="15">
-        <v>10221535</v>
+        <v>9683569</v>
       </c>
     </row>
     <row r="52" spans="1:11">
       <c r="A52" s="16" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B52" s="15" t="s">
         <v>446</v>
@@ -4750,13 +4769,13 @@
         <v>89</v>
       </c>
       <c r="F52" s="16" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G52" s="15">
-        <v>1992</v>
+        <v>1996</v>
       </c>
       <c r="H52" s="16" t="s">
-        <v>99</v>
+        <v>42</v>
       </c>
       <c r="I52" s="16" t="s">
         <v>435</v>
@@ -4765,12 +4784,12 @@
         <v>316</v>
       </c>
       <c r="K52" s="15">
-        <v>9621027</v>
+        <v>10221535</v>
       </c>
     </row>
     <row r="53" spans="1:11">
       <c r="A53" s="16" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B53" s="15" t="s">
         <v>446</v>
@@ -4782,16 +4801,16 @@
         <v>374</v>
       </c>
       <c r="E53" s="16" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="F53" s="16" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="G53" s="15">
-        <v>1990</v>
+        <v>1992</v>
       </c>
       <c r="H53" s="16" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="I53" s="16" t="s">
         <v>435</v>
@@ -4800,12 +4819,12 @@
         <v>316</v>
       </c>
       <c r="K53" s="15">
-        <v>9621028</v>
+        <v>9621027</v>
       </c>
     </row>
     <row r="54" spans="1:11">
       <c r="A54" s="16" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B54" s="15" t="s">
         <v>446</v>
@@ -4820,13 +4839,13 @@
         <v>101</v>
       </c>
       <c r="F54" s="16" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G54" s="15">
-        <v>1994</v>
+        <v>1990</v>
       </c>
       <c r="H54" s="16" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="I54" s="16" t="s">
         <v>435</v>
@@ -4835,12 +4854,12 @@
         <v>316</v>
       </c>
       <c r="K54" s="15">
-        <v>10983640</v>
+        <v>9621028</v>
       </c>
     </row>
     <row r="55" spans="1:11">
       <c r="A55" s="16" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B55" s="15" t="s">
         <v>446</v>
@@ -4855,10 +4874,10 @@
         <v>101</v>
       </c>
       <c r="F55" s="16" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="G55" s="15">
-        <v>1993</v>
+        <v>1994</v>
       </c>
       <c r="H55" s="16" t="s">
         <v>106</v>
@@ -4870,12 +4889,12 @@
         <v>316</v>
       </c>
       <c r="K55" s="15">
-        <v>10983641</v>
+        <v>10983640</v>
       </c>
     </row>
     <row r="56" spans="1:11">
       <c r="A56" s="16" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B56" s="15" t="s">
         <v>446</v>
@@ -4887,16 +4906,16 @@
         <v>374</v>
       </c>
       <c r="E56" s="16" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="F56" s="16" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="G56" s="15">
-        <v>1994</v>
+        <v>1993</v>
       </c>
       <c r="H56" s="16" t="s">
-        <v>91</v>
+        <v>106</v>
       </c>
       <c r="I56" s="16" t="s">
         <v>435</v>
@@ -4905,12 +4924,12 @@
         <v>316</v>
       </c>
       <c r="K56" s="15">
-        <v>10052760</v>
+        <v>10983641</v>
       </c>
     </row>
     <row r="57" spans="1:11">
       <c r="A57" s="16" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B57" s="15" t="s">
         <v>446</v>
@@ -4925,10 +4944,10 @@
         <v>110</v>
       </c>
       <c r="F57" s="16" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G57" s="15">
-        <v>1993</v>
+        <v>1994</v>
       </c>
       <c r="H57" s="16" t="s">
         <v>91</v>
@@ -4940,12 +4959,12 @@
         <v>316</v>
       </c>
       <c r="K57" s="15">
-        <v>10052761</v>
+        <v>10052760</v>
       </c>
     </row>
     <row r="58" spans="1:11">
       <c r="A58" s="16" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B58" s="15" t="s">
         <v>446</v>
@@ -4957,16 +4976,16 @@
         <v>374</v>
       </c>
       <c r="E58" s="16" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="F58" s="16" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="G58" s="15">
-        <v>1997</v>
+        <v>1993</v>
       </c>
       <c r="H58" s="16" t="s">
-        <v>42</v>
+        <v>91</v>
       </c>
       <c r="I58" s="16" t="s">
         <v>435</v>
@@ -4975,12 +4994,12 @@
         <v>316</v>
       </c>
       <c r="K58" s="15">
-        <v>10659053</v>
+        <v>10052761</v>
       </c>
     </row>
     <row r="59" spans="1:11">
       <c r="A59" s="16" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B59" s="15" t="s">
         <v>446</v>
@@ -4995,13 +5014,13 @@
         <v>115</v>
       </c>
       <c r="F59" s="16" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G59" s="15">
-        <v>1996</v>
+        <v>1997</v>
       </c>
       <c r="H59" s="16" t="s">
-        <v>66</v>
+        <v>42</v>
       </c>
       <c r="I59" s="16" t="s">
         <v>435</v>
@@ -5010,12 +5029,12 @@
         <v>316</v>
       </c>
       <c r="K59" s="15">
-        <v>10659054</v>
+        <v>10659053</v>
       </c>
     </row>
     <row r="60" spans="1:11">
-      <c r="A60" s="15" t="s">
-        <v>173</v>
+      <c r="A60" s="16" t="s">
+        <v>117</v>
       </c>
       <c r="B60" s="15" t="s">
         <v>446</v>
@@ -5024,16 +5043,18 @@
         <v>348</v>
       </c>
       <c r="D60" s="15" t="s">
-        <v>376</v>
-      </c>
-      <c r="E60" s="15"/>
-      <c r="F60" s="15" t="s">
-        <v>264</v>
+        <v>374</v>
+      </c>
+      <c r="E60" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="F60" s="16" t="s">
+        <v>118</v>
       </c>
       <c r="G60" s="15">
-        <v>2002</v>
-      </c>
-      <c r="H60" s="15" t="s">
+        <v>1996</v>
+      </c>
+      <c r="H60" s="16" t="s">
         <v>66</v>
       </c>
       <c r="I60" s="16" t="s">
@@ -5042,11 +5063,13 @@
       <c r="J60" s="16" t="s">
         <v>316</v>
       </c>
-      <c r="K60" s="15"/>
+      <c r="K60" s="15">
+        <v>10659054</v>
+      </c>
     </row>
     <row r="61" spans="1:11">
       <c r="A61" s="15" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B61" s="15" t="s">
         <v>446</v>
@@ -5059,10 +5082,10 @@
       </c>
       <c r="E61" s="15"/>
       <c r="F61" s="15" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="G61" s="15">
-        <v>2004</v>
+        <v>2002</v>
       </c>
       <c r="H61" s="15" t="s">
         <v>66</v>
@@ -5077,7 +5100,7 @@
     </row>
     <row r="62" spans="1:11">
       <c r="A62" s="15" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B62" s="15" t="s">
         <v>446</v>
@@ -5090,7 +5113,7 @@
       </c>
       <c r="E62" s="15"/>
       <c r="F62" s="15" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G62" s="15">
         <v>2004</v>
@@ -5108,7 +5131,7 @@
     </row>
     <row r="63" spans="1:11">
       <c r="A63" s="15" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B63" s="15" t="s">
         <v>446</v>
@@ -5121,10 +5144,10 @@
       </c>
       <c r="E63" s="15"/>
       <c r="F63" s="15" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G63" s="15">
-        <v>1995</v>
+        <v>2004</v>
       </c>
       <c r="H63" s="15" t="s">
         <v>66</v>
@@ -5139,7 +5162,7 @@
     </row>
     <row r="64" spans="1:11">
       <c r="A64" s="15" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B64" s="15" t="s">
         <v>446</v>
@@ -5148,14 +5171,14 @@
         <v>348</v>
       </c>
       <c r="D64" s="15" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E64" s="15"/>
       <c r="F64" s="15" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="G64" s="15">
-        <v>1991</v>
+        <v>1995</v>
       </c>
       <c r="H64" s="15" t="s">
         <v>66</v>
@@ -5170,7 +5193,7 @@
     </row>
     <row r="65" spans="1:11">
       <c r="A65" s="15" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B65" s="15" t="s">
         <v>446</v>
@@ -5183,10 +5206,10 @@
       </c>
       <c r="E65" s="15"/>
       <c r="F65" s="15" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G65" s="15">
-        <v>1998</v>
+        <v>1991</v>
       </c>
       <c r="H65" s="15" t="s">
         <v>66</v>
@@ -5201,7 +5224,7 @@
     </row>
     <row r="66" spans="1:11">
       <c r="A66" s="15" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B66" s="15" t="s">
         <v>446</v>
@@ -5214,7 +5237,7 @@
       </c>
       <c r="E66" s="15"/>
       <c r="F66" s="15" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G66" s="15">
         <v>1998</v>
@@ -5232,7 +5255,7 @@
     </row>
     <row r="67" spans="1:11">
       <c r="A67" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B67" s="15" t="s">
         <v>446</v>
@@ -5245,13 +5268,13 @@
       </c>
       <c r="E67" s="15"/>
       <c r="F67" s="15" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="G67" s="15">
-        <v>1999</v>
+        <v>1998</v>
       </c>
       <c r="H67" s="15" t="s">
-        <v>317</v>
+        <v>66</v>
       </c>
       <c r="I67" s="16" t="s">
         <v>435</v>
@@ -5263,7 +5286,7 @@
     </row>
     <row r="68" spans="1:11">
       <c r="A68" s="15" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B68" s="15" t="s">
         <v>446</v>
@@ -5276,13 +5299,13 @@
       </c>
       <c r="E68" s="15"/>
       <c r="F68" s="15" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="G68" s="15">
         <v>1999</v>
       </c>
       <c r="H68" s="15" t="s">
-        <v>19</v>
+        <v>317</v>
       </c>
       <c r="I68" s="16" t="s">
         <v>435</v>
@@ -5294,26 +5317,26 @@
     </row>
     <row r="69" spans="1:11">
       <c r="A69" s="15" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B69" s="15" t="s">
         <v>446</v>
       </c>
-      <c r="C69" s="15" t="s">
+      <c r="C69" s="16" t="s">
         <v>348</v>
       </c>
       <c r="D69" s="15" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="E69" s="15"/>
       <c r="F69" s="15" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G69" s="15">
-        <v>2006</v>
+        <v>1999</v>
       </c>
       <c r="H69" s="15" t="s">
-        <v>66</v>
+        <v>19</v>
       </c>
       <c r="I69" s="16" t="s">
         <v>435</v>
@@ -5325,26 +5348,26 @@
     </row>
     <row r="70" spans="1:11">
       <c r="A70" s="15" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="B70" s="15" t="s">
         <v>446</v>
       </c>
       <c r="C70" s="15" t="s">
-        <v>379</v>
+        <v>348</v>
       </c>
       <c r="D70" s="15" t="s">
-        <v>14</v>
+        <v>380</v>
       </c>
       <c r="E70" s="15"/>
       <c r="F70" s="15" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="G70" s="15">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="H70" s="15" t="s">
-        <v>321</v>
+        <v>66</v>
       </c>
       <c r="I70" s="16" t="s">
         <v>435</v>
@@ -5356,7 +5379,7 @@
     </row>
     <row r="71" spans="1:11">
       <c r="A71" s="15" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="B71" s="15" t="s">
         <v>446</v>
@@ -5365,17 +5388,17 @@
         <v>379</v>
       </c>
       <c r="D71" s="15" t="s">
-        <v>454</v>
+        <v>14</v>
       </c>
       <c r="E71" s="15"/>
       <c r="F71" s="15" t="s">
-        <v>275</v>
-      </c>
-      <c r="G71" s="15" t="s">
-        <v>14</v>
+        <v>281</v>
+      </c>
+      <c r="G71" s="15">
+        <v>2007</v>
       </c>
       <c r="H71" s="15" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="I71" s="16" t="s">
         <v>435</v>
@@ -5387,7 +5410,7 @@
     </row>
     <row r="72" spans="1:11">
       <c r="A72" s="15" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B72" s="15" t="s">
         <v>446</v>
@@ -5400,13 +5423,13 @@
       </c>
       <c r="E72" s="15"/>
       <c r="F72" s="15" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G72" s="15" t="s">
         <v>14</v>
       </c>
       <c r="H72" s="15" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="I72" s="16" t="s">
         <v>435</v>
@@ -5418,7 +5441,7 @@
     </row>
     <row r="73" spans="1:11">
       <c r="A73" s="15" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B73" s="15" t="s">
         <v>446</v>
@@ -5431,13 +5454,13 @@
       </c>
       <c r="E73" s="15"/>
       <c r="F73" s="15" t="s">
-        <v>277</v>
-      </c>
-      <c r="G73" s="15">
-        <v>1986</v>
+        <v>276</v>
+      </c>
+      <c r="G73" s="15" t="s">
+        <v>14</v>
       </c>
       <c r="H73" s="15" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="I73" s="16" t="s">
         <v>435</v>
@@ -5449,7 +5472,7 @@
     </row>
     <row r="74" spans="1:11">
       <c r="A74" s="15" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B74" s="15" t="s">
         <v>446</v>
@@ -5458,17 +5481,17 @@
         <v>379</v>
       </c>
       <c r="D74" s="15" t="s">
-        <v>8</v>
+        <v>454</v>
       </c>
       <c r="E74" s="15"/>
       <c r="F74" s="15" t="s">
-        <v>278</v>
-      </c>
-      <c r="G74" s="15" t="s">
-        <v>14</v>
+        <v>277</v>
+      </c>
+      <c r="G74" s="15">
+        <v>1986</v>
       </c>
       <c r="H74" s="15" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="I74" s="16" t="s">
         <v>435</v>
@@ -5480,7 +5503,7 @@
     </row>
     <row r="75" spans="1:11">
       <c r="A75" s="15" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B75" s="15" t="s">
         <v>446</v>
@@ -5493,13 +5516,13 @@
       </c>
       <c r="E75" s="15"/>
       <c r="F75" s="15" t="s">
-        <v>279</v>
-      </c>
-      <c r="G75" s="15">
-        <v>1986</v>
+        <v>278</v>
+      </c>
+      <c r="G75" s="15" t="s">
+        <v>14</v>
       </c>
       <c r="H75" s="15" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="I75" s="16" t="s">
         <v>435</v>
@@ -5511,7 +5534,7 @@
     </row>
     <row r="76" spans="1:11">
       <c r="A76" s="15" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B76" s="15" t="s">
         <v>446</v>
@@ -5520,17 +5543,17 @@
         <v>379</v>
       </c>
       <c r="D76" s="15" t="s">
-        <v>89</v>
+        <v>8</v>
       </c>
       <c r="E76" s="15"/>
       <c r="F76" s="15" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="G76" s="15">
-        <v>1992</v>
+        <v>1986</v>
       </c>
       <c r="H76" s="15" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="I76" s="16" t="s">
         <v>435</v>
@@ -5542,7 +5565,7 @@
     </row>
     <row r="77" spans="1:11">
       <c r="A77" s="15" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B77" s="15" t="s">
         <v>446</v>
@@ -5551,17 +5574,17 @@
         <v>379</v>
       </c>
       <c r="D77" s="15" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="E77" s="15"/>
-      <c r="F77" s="15">
-        <v>12034</v>
+      <c r="F77" s="15" t="s">
+        <v>280</v>
       </c>
       <c r="G77" s="15">
-        <v>1996</v>
+        <v>1992</v>
       </c>
       <c r="H77" s="15" t="s">
-        <v>10</v>
+        <v>321</v>
       </c>
       <c r="I77" s="16" t="s">
         <v>435</v>
@@ -5572,39 +5595,39 @@
       <c r="K77" s="15"/>
     </row>
     <row r="78" spans="1:11">
-      <c r="A78" s="17" t="s">
-        <v>202</v>
-      </c>
-      <c r="B78" s="18" t="s">
-        <v>446</v>
-      </c>
-      <c r="C78" s="17" t="s">
-        <v>352</v>
-      </c>
-      <c r="D78" s="15"/>
-      <c r="E78" s="17" t="s">
-        <v>498</v>
-      </c>
-      <c r="F78" s="15" t="s">
-        <v>290</v>
+      <c r="A78" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="B78" s="15" t="s">
+        <v>446</v>
+      </c>
+      <c r="C78" s="15" t="s">
+        <v>379</v>
+      </c>
+      <c r="D78" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="E78" s="15"/>
+      <c r="F78" s="15">
+        <v>12034</v>
       </c>
       <c r="G78" s="15">
-        <v>1999</v>
+        <v>1996</v>
       </c>
       <c r="H78" s="15" t="s">
-        <v>66</v>
+        <v>10</v>
       </c>
       <c r="I78" s="16" t="s">
-        <v>422</v>
+        <v>435</v>
       </c>
       <c r="J78" s="16" t="s">
-        <v>403</v>
-      </c>
-      <c r="K78" s="16"/>
+        <v>316</v>
+      </c>
+      <c r="K78" s="15"/>
     </row>
     <row r="79" spans="1:11">
       <c r="A79" s="17" t="s">
-        <v>224</v>
+        <v>202</v>
       </c>
       <c r="B79" s="18" t="s">
         <v>446</v>
@@ -5617,25 +5640,25 @@
         <v>498</v>
       </c>
       <c r="F79" s="15" t="s">
-        <v>310</v>
-      </c>
-      <c r="G79" s="15" t="s">
-        <v>14</v>
+        <v>290</v>
+      </c>
+      <c r="G79" s="15">
+        <v>1999</v>
       </c>
       <c r="H79" s="15" t="s">
-        <v>33</v>
+        <v>66</v>
       </c>
       <c r="I79" s="16" t="s">
-        <v>375</v>
+        <v>422</v>
       </c>
       <c r="J79" s="16" t="s">
-        <v>425</v>
+        <v>403</v>
       </c>
       <c r="K79" s="16"/>
     </row>
     <row r="80" spans="1:11">
       <c r="A80" s="17" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B80" s="18" t="s">
         <v>446</v>
@@ -5648,13 +5671,13 @@
         <v>498</v>
       </c>
       <c r="F80" s="15" t="s">
-        <v>311</v>
-      </c>
-      <c r="G80" s="15">
-        <v>2010</v>
+        <v>310</v>
+      </c>
+      <c r="G80" s="15" t="s">
+        <v>14</v>
       </c>
       <c r="H80" s="15" t="s">
-        <v>362</v>
+        <v>33</v>
       </c>
       <c r="I80" s="16" t="s">
         <v>375</v>
@@ -5666,7 +5689,7 @@
     </row>
     <row r="81" spans="1:11">
       <c r="A81" s="17" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B81" s="18" t="s">
         <v>446</v>
@@ -5679,7 +5702,7 @@
         <v>498</v>
       </c>
       <c r="F81" s="15" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="G81" s="15">
         <v>2010</v>
@@ -5697,7 +5720,7 @@
     </row>
     <row r="82" spans="1:11">
       <c r="A82" s="17" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B82" s="18" t="s">
         <v>446</v>
@@ -5710,7 +5733,7 @@
         <v>498</v>
       </c>
       <c r="F82" s="15" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="G82" s="15">
         <v>2010</v>
@@ -5728,7 +5751,7 @@
     </row>
     <row r="83" spans="1:11">
       <c r="A83" s="17" t="s">
-        <v>351</v>
+        <v>227</v>
       </c>
       <c r="B83" s="18" t="s">
         <v>446</v>
@@ -5740,146 +5763,146 @@
       <c r="E83" s="17" t="s">
         <v>498</v>
       </c>
-      <c r="F83" s="16" t="s">
-        <v>352</v>
-      </c>
-      <c r="G83" s="15"/>
-      <c r="H83" s="16"/>
+      <c r="F83" s="15" t="s">
+        <v>313</v>
+      </c>
+      <c r="G83" s="15">
+        <v>2010</v>
+      </c>
+      <c r="H83" s="15" t="s">
+        <v>362</v>
+      </c>
       <c r="I83" s="16" t="s">
-        <v>363</v>
+        <v>375</v>
       </c>
       <c r="J83" s="16" t="s">
-        <v>402</v>
+        <v>425</v>
       </c>
       <c r="K83" s="16"/>
     </row>
     <row r="84" spans="1:11">
       <c r="A84" s="17" t="s">
-        <v>169</v>
+        <v>351</v>
       </c>
       <c r="B84" s="18" t="s">
         <v>446</v>
       </c>
       <c r="C84" s="17" t="s">
-        <v>469</v>
+        <v>352</v>
       </c>
       <c r="D84" s="15"/>
       <c r="E84" s="17" t="s">
-        <v>499</v>
-      </c>
-      <c r="F84" s="15" t="s">
-        <v>260</v>
-      </c>
-      <c r="G84" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="H84" s="15" t="s">
-        <v>49</v>
-      </c>
+        <v>498</v>
+      </c>
+      <c r="F84" s="16" t="s">
+        <v>352</v>
+      </c>
+      <c r="G84" s="15"/>
+      <c r="H84" s="16"/>
       <c r="I84" s="16" t="s">
-        <v>416</v>
+        <v>363</v>
       </c>
       <c r="J84" s="16" t="s">
-        <v>396</v>
+        <v>402</v>
       </c>
       <c r="K84" s="16"/>
     </row>
     <row r="85" spans="1:11">
       <c r="A85" s="17" t="s">
-        <v>196</v>
+        <v>169</v>
       </c>
       <c r="B85" s="18" t="s">
         <v>446</v>
       </c>
       <c r="C85" s="17" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="D85" s="15"/>
       <c r="E85" s="17" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="F85" s="15" t="s">
-        <v>285</v>
-      </c>
-      <c r="G85" s="15">
-        <v>2009</v>
+        <v>260</v>
+      </c>
+      <c r="G85" s="15" t="s">
+        <v>14</v>
       </c>
       <c r="H85" s="15" t="s">
-        <v>362</v>
+        <v>49</v>
       </c>
       <c r="I85" s="16" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="J85" s="16" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="K85" s="16"/>
     </row>
     <row r="86" spans="1:11">
       <c r="A86" s="17" t="s">
-        <v>223</v>
+        <v>196</v>
       </c>
       <c r="B86" s="18" t="s">
         <v>446</v>
       </c>
       <c r="C86" s="17" t="s">
-        <v>459</v>
+        <v>470</v>
       </c>
       <c r="D86" s="15"/>
       <c r="E86" s="17" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="F86" s="15" t="s">
-        <v>309</v>
-      </c>
-      <c r="G86" s="15" t="s">
-        <v>14</v>
+        <v>285</v>
+      </c>
+      <c r="G86" s="15">
+        <v>2009</v>
       </c>
       <c r="H86" s="15" t="s">
-        <v>30</v>
+        <v>362</v>
       </c>
       <c r="I86" s="16" t="s">
-        <v>368</v>
+        <v>420</v>
       </c>
       <c r="J86" s="16" t="s">
-        <v>424</v>
+        <v>400</v>
       </c>
       <c r="K86" s="16"/>
     </row>
     <row r="87" spans="1:11">
       <c r="A87" s="17" t="s">
-        <v>143</v>
+        <v>223</v>
       </c>
       <c r="B87" s="18" t="s">
         <v>446</v>
       </c>
       <c r="C87" s="17" t="s">
-        <v>455</v>
+        <v>459</v>
       </c>
       <c r="D87" s="15"/>
       <c r="E87" s="17" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="F87" s="15" t="s">
-        <v>234</v>
+        <v>309</v>
       </c>
       <c r="G87" s="15" t="s">
         <v>14</v>
       </c>
       <c r="H87" s="15" t="s">
-        <v>66</v>
+        <v>30</v>
       </c>
       <c r="I87" s="16" t="s">
-        <v>412</v>
+        <v>368</v>
       </c>
       <c r="J87" s="16" t="s">
-        <v>393</v>
+        <v>424</v>
       </c>
       <c r="K87" s="16"/>
     </row>
-    <row r="88" spans="1:11" ht="13" customHeight="1">
+    <row r="88" spans="1:11">
       <c r="A88" s="17" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B88" s="18" t="s">
         <v>446</v>
@@ -5892,13 +5915,13 @@
         <v>502</v>
       </c>
       <c r="F88" s="15" t="s">
-        <v>235</v>
-      </c>
-      <c r="G88" s="15">
-        <v>2010</v>
+        <v>234</v>
+      </c>
+      <c r="G88" s="15" t="s">
+        <v>14</v>
       </c>
       <c r="H88" s="15" t="s">
-        <v>30</v>
+        <v>66</v>
       </c>
       <c r="I88" s="16" t="s">
         <v>412</v>
@@ -5908,9 +5931,9 @@
       </c>
       <c r="K88" s="16"/>
     </row>
-    <row r="89" spans="1:11">
+    <row r="89" spans="1:11" ht="13" customHeight="1">
       <c r="A89" s="17" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B89" s="18" t="s">
         <v>446</v>
@@ -5923,7 +5946,7 @@
         <v>502</v>
       </c>
       <c r="F89" s="15" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G89" s="15">
         <v>2010</v>
@@ -5941,38 +5964,38 @@
     </row>
     <row r="90" spans="1:11">
       <c r="A90" s="17" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B90" s="18" t="s">
         <v>446</v>
       </c>
       <c r="C90" s="17" t="s">
-        <v>354</v>
+        <v>455</v>
       </c>
       <c r="D90" s="15"/>
       <c r="E90" s="17" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="F90" s="15" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G90" s="15">
-        <v>2006</v>
+        <v>2010</v>
       </c>
       <c r="H90" s="15" t="s">
-        <v>440</v>
+        <v>30</v>
       </c>
       <c r="I90" s="16" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="J90" s="16" t="s">
-        <v>465</v>
+        <v>393</v>
       </c>
       <c r="K90" s="16"/>
     </row>
     <row r="91" spans="1:11">
       <c r="A91" s="17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B91" s="18" t="s">
         <v>446</v>
@@ -5985,10 +6008,10 @@
         <v>503</v>
       </c>
       <c r="F91" s="15" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G91" s="15">
-        <v>1990</v>
+        <v>2006</v>
       </c>
       <c r="H91" s="15" t="s">
         <v>440</v>
@@ -6003,7 +6026,7 @@
     </row>
     <row r="92" spans="1:11">
       <c r="A92" s="17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B92" s="18" t="s">
         <v>446</v>
@@ -6016,13 +6039,13 @@
         <v>503</v>
       </c>
       <c r="F92" s="15" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G92" s="15">
-        <v>2001</v>
+        <v>1990</v>
       </c>
       <c r="H92" s="15" t="s">
-        <v>66</v>
+        <v>440</v>
       </c>
       <c r="I92" s="16" t="s">
         <v>413</v>
@@ -6034,7 +6057,7 @@
     </row>
     <row r="93" spans="1:11">
       <c r="A93" s="17" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B93" s="18" t="s">
         <v>446</v>
@@ -6047,10 +6070,10 @@
         <v>503</v>
       </c>
       <c r="F93" s="15" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G93" s="15">
-        <v>2005</v>
+        <v>2001</v>
       </c>
       <c r="H93" s="15" t="s">
         <v>66</v>
@@ -6065,7 +6088,7 @@
     </row>
     <row r="94" spans="1:11">
       <c r="A94" s="17" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B94" s="18" t="s">
         <v>446</v>
@@ -6078,7 +6101,7 @@
         <v>503</v>
       </c>
       <c r="F94" s="15" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G94" s="15">
         <v>2005</v>
@@ -6096,7 +6119,7 @@
     </row>
     <row r="95" spans="1:11">
       <c r="A95" s="17" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B95" s="18" t="s">
         <v>446</v>
@@ -6109,7 +6132,7 @@
         <v>503</v>
       </c>
       <c r="F95" s="15" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G95" s="15">
         <v>2005</v>
@@ -6127,7 +6150,7 @@
     </row>
     <row r="96" spans="1:11">
       <c r="A96" s="17" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B96" s="18" t="s">
         <v>446</v>
@@ -6140,7 +6163,7 @@
         <v>503</v>
       </c>
       <c r="F96" s="15" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G96" s="15">
         <v>2005</v>
@@ -6158,7 +6181,7 @@
     </row>
     <row r="97" spans="1:11">
       <c r="A97" s="17" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B97" s="18" t="s">
         <v>446</v>
@@ -6171,7 +6194,7 @@
         <v>503</v>
       </c>
       <c r="F97" s="15" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G97" s="15">
         <v>2005</v>
@@ -6189,7 +6212,7 @@
     </row>
     <row r="98" spans="1:11">
       <c r="A98" s="17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B98" s="18" t="s">
         <v>446</v>
@@ -6202,7 +6225,7 @@
         <v>503</v>
       </c>
       <c r="F98" s="15" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G98" s="15">
         <v>2005</v>
@@ -6220,7 +6243,7 @@
     </row>
     <row r="99" spans="1:11">
       <c r="A99" s="17" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B99" s="18" t="s">
         <v>446</v>
@@ -6233,13 +6256,13 @@
         <v>503</v>
       </c>
       <c r="F99" s="15" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G99" s="15">
-        <v>1988</v>
+        <v>2005</v>
       </c>
       <c r="H99" s="15" t="s">
-        <v>361</v>
+        <v>66</v>
       </c>
       <c r="I99" s="16" t="s">
         <v>413</v>
@@ -6251,7 +6274,7 @@
     </row>
     <row r="100" spans="1:11">
       <c r="A100" s="17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B100" s="18" t="s">
         <v>446</v>
@@ -6264,13 +6287,13 @@
         <v>503</v>
       </c>
       <c r="F100" s="15" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G100" s="15">
-        <v>2000</v>
+        <v>1988</v>
       </c>
       <c r="H100" s="15" t="s">
-        <v>69</v>
+        <v>361</v>
       </c>
       <c r="I100" s="16" t="s">
         <v>413</v>
@@ -6282,7 +6305,7 @@
     </row>
     <row r="101" spans="1:11">
       <c r="A101" s="17" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B101" s="18" t="s">
         <v>446</v>
@@ -6295,10 +6318,10 @@
         <v>503</v>
       </c>
       <c r="F101" s="15" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G101" s="15">
-        <v>2006</v>
+        <v>2000</v>
       </c>
       <c r="H101" s="15" t="s">
         <v>69</v>
@@ -6313,7 +6336,7 @@
     </row>
     <row r="102" spans="1:11">
       <c r="A102" s="17" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B102" s="18" t="s">
         <v>446</v>
@@ -6326,10 +6349,10 @@
         <v>503</v>
       </c>
       <c r="F102" s="15" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G102" s="15">
-        <v>2009</v>
+        <v>2006</v>
       </c>
       <c r="H102" s="15" t="s">
         <v>69</v>
@@ -6344,7 +6367,7 @@
     </row>
     <row r="103" spans="1:11">
       <c r="A103" s="17" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B103" s="18" t="s">
         <v>446</v>
@@ -6357,13 +6380,13 @@
         <v>503</v>
       </c>
       <c r="F103" s="15" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G103" s="15">
-        <v>1985</v>
+        <v>2009</v>
       </c>
       <c r="H103" s="15" t="s">
-        <v>441</v>
+        <v>69</v>
       </c>
       <c r="I103" s="16" t="s">
         <v>413</v>
@@ -6375,7 +6398,7 @@
     </row>
     <row r="104" spans="1:11">
       <c r="A104" s="17" t="s">
-        <v>353</v>
+        <v>159</v>
       </c>
       <c r="B104" s="18" t="s">
         <v>446</v>
@@ -6387,13 +6410,17 @@
       <c r="E104" s="17" t="s">
         <v>503</v>
       </c>
-      <c r="F104" s="16" t="s">
-        <v>354</v>
-      </c>
-      <c r="G104" s="15"/>
-      <c r="H104" s="16"/>
+      <c r="F104" s="15" t="s">
+        <v>250</v>
+      </c>
+      <c r="G104" s="15">
+        <v>1985</v>
+      </c>
+      <c r="H104" s="15" t="s">
+        <v>441</v>
+      </c>
       <c r="I104" s="16" t="s">
-        <v>389</v>
+        <v>413</v>
       </c>
       <c r="J104" s="16" t="s">
         <v>465</v>
@@ -6402,7 +6429,7 @@
     </row>
     <row r="105" spans="1:11">
       <c r="A105" s="17" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B105" s="18" t="s">
         <v>446</v>
@@ -6415,7 +6442,7 @@
         <v>503</v>
       </c>
       <c r="F105" s="16" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="G105" s="15"/>
       <c r="H105" s="16"/>
@@ -6429,38 +6456,34 @@
     </row>
     <row r="106" spans="1:11">
       <c r="A106" s="17" t="s">
-        <v>160</v>
+        <v>355</v>
       </c>
       <c r="B106" s="18" t="s">
         <v>446</v>
       </c>
       <c r="C106" s="17" t="s">
-        <v>464</v>
+        <v>354</v>
       </c>
       <c r="D106" s="15"/>
       <c r="E106" s="17" t="s">
-        <v>504</v>
-      </c>
-      <c r="F106" s="15" t="s">
-        <v>251</v>
-      </c>
-      <c r="G106" s="15">
-        <v>2004</v>
-      </c>
-      <c r="H106" s="15" t="s">
-        <v>66</v>
-      </c>
+        <v>503</v>
+      </c>
+      <c r="F106" s="16" t="s">
+        <v>356</v>
+      </c>
+      <c r="G106" s="15"/>
+      <c r="H106" s="16"/>
       <c r="I106" s="16" t="s">
-        <v>414</v>
+        <v>389</v>
       </c>
       <c r="J106" s="16" t="s">
-        <v>394</v>
+        <v>465</v>
       </c>
       <c r="K106" s="16"/>
     </row>
     <row r="107" spans="1:11">
       <c r="A107" s="17" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B107" s="18" t="s">
         <v>446</v>
@@ -6473,10 +6496,10 @@
         <v>504</v>
       </c>
       <c r="F107" s="15" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G107" s="15">
-        <v>1999</v>
+        <v>2004</v>
       </c>
       <c r="H107" s="15" t="s">
         <v>66</v>
@@ -6491,7 +6514,7 @@
     </row>
     <row r="108" spans="1:11">
       <c r="A108" s="17" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B108" s="18" t="s">
         <v>446</v>
@@ -6504,7 +6527,7 @@
         <v>504</v>
       </c>
       <c r="F108" s="15" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G108" s="15">
         <v>1999</v>
@@ -6522,92 +6545,92 @@
     </row>
     <row r="109" spans="1:11">
       <c r="A109" s="17" t="s">
-        <v>357</v>
+        <v>162</v>
       </c>
       <c r="B109" s="18" t="s">
         <v>446</v>
       </c>
       <c r="C109" s="17" t="s">
-        <v>358</v>
+        <v>464</v>
       </c>
       <c r="D109" s="15"/>
       <c r="E109" s="17" t="s">
-        <v>505</v>
-      </c>
-      <c r="F109" s="16" t="s">
-        <v>358</v>
-      </c>
-      <c r="G109" s="15"/>
-      <c r="H109" s="16"/>
+        <v>504</v>
+      </c>
+      <c r="F109" s="15" t="s">
+        <v>253</v>
+      </c>
+      <c r="G109" s="15">
+        <v>1999</v>
+      </c>
+      <c r="H109" s="15" t="s">
+        <v>66</v>
+      </c>
       <c r="I109" s="16" t="s">
-        <v>390</v>
+        <v>414</v>
       </c>
       <c r="J109" s="16" t="s">
-        <v>428</v>
+        <v>394</v>
       </c>
       <c r="K109" s="16"/>
     </row>
     <row r="110" spans="1:11">
       <c r="A110" s="17" t="s">
-        <v>349</v>
+        <v>357</v>
       </c>
       <c r="B110" s="18" t="s">
         <v>446</v>
       </c>
       <c r="C110" s="17" t="s">
-        <v>350</v>
+        <v>358</v>
       </c>
       <c r="D110" s="15"/>
       <c r="E110" s="17" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="F110" s="16" t="s">
-        <v>350</v>
+        <v>358</v>
       </c>
       <c r="G110" s="15"/>
       <c r="H110" s="16"/>
       <c r="I110" s="16" t="s">
-        <v>447</v>
+        <v>390</v>
       </c>
       <c r="J110" s="16" t="s">
-        <v>461</v>
+        <v>428</v>
       </c>
       <c r="K110" s="16"/>
     </row>
     <row r="111" spans="1:11">
       <c r="A111" s="17" t="s">
-        <v>163</v>
+        <v>349</v>
       </c>
       <c r="B111" s="18" t="s">
         <v>446</v>
       </c>
       <c r="C111" s="17" t="s">
-        <v>456</v>
+        <v>350</v>
       </c>
       <c r="D111" s="15"/>
       <c r="E111" s="17" t="s">
-        <v>507</v>
-      </c>
-      <c r="F111" s="15" t="s">
-        <v>254</v>
-      </c>
-      <c r="G111" s="15">
-        <v>2004</v>
-      </c>
-      <c r="H111" s="15" t="s">
-        <v>66</v>
-      </c>
+        <v>506</v>
+      </c>
+      <c r="F111" s="16" t="s">
+        <v>350</v>
+      </c>
+      <c r="G111" s="15"/>
+      <c r="H111" s="16"/>
       <c r="I111" s="16" t="s">
-        <v>415</v>
+        <v>447</v>
       </c>
       <c r="J111" s="16" t="s">
-        <v>395</v>
+        <v>461</v>
       </c>
       <c r="K111" s="16"/>
     </row>
     <row r="112" spans="1:11">
       <c r="A112" s="17" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B112" s="18" t="s">
         <v>446</v>
@@ -6620,10 +6643,10 @@
         <v>507</v>
       </c>
       <c r="F112" s="15" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G112" s="15">
-        <v>2007</v>
+        <v>2004</v>
       </c>
       <c r="H112" s="15" t="s">
         <v>66</v>
@@ -6638,7 +6661,7 @@
     </row>
     <row r="113" spans="1:11">
       <c r="A113" s="17" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B113" s="18" t="s">
         <v>446</v>
@@ -6651,7 +6674,7 @@
         <v>507</v>
       </c>
       <c r="F113" s="15" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G113" s="15">
         <v>2007</v>
@@ -6669,7 +6692,7 @@
     </row>
     <row r="114" spans="1:11">
       <c r="A114" s="17" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B114" s="18" t="s">
         <v>446</v>
@@ -6682,10 +6705,10 @@
         <v>507</v>
       </c>
       <c r="F114" s="15" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G114" s="15">
-        <v>2012</v>
+        <v>2007</v>
       </c>
       <c r="H114" s="15" t="s">
         <v>66</v>
@@ -6700,7 +6723,7 @@
     </row>
     <row r="115" spans="1:11">
       <c r="A115" s="17" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B115" s="18" t="s">
         <v>446</v>
@@ -6713,7 +6736,7 @@
         <v>507</v>
       </c>
       <c r="F115" s="15" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="G115" s="15">
         <v>2012</v>
@@ -6731,7 +6754,7 @@
     </row>
     <row r="116" spans="1:11">
       <c r="A116" s="17" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B116" s="18" t="s">
         <v>446</v>
@@ -6744,10 +6767,10 @@
         <v>507</v>
       </c>
       <c r="F116" s="15" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="G116" s="15">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="H116" s="15" t="s">
         <v>66</v>
@@ -6762,38 +6785,38 @@
     </row>
     <row r="117" spans="1:11">
       <c r="A117" s="17" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B117" s="18" t="s">
         <v>446</v>
       </c>
       <c r="C117" s="17" t="s">
-        <v>468</v>
+        <v>456</v>
       </c>
       <c r="D117" s="15"/>
       <c r="E117" s="17" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="F117" s="15" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="G117" s="15">
-        <v>1999</v>
+        <v>2013</v>
       </c>
       <c r="H117" s="15" t="s">
         <v>66</v>
       </c>
       <c r="I117" s="16" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="J117" s="16" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="K117" s="16"/>
     </row>
     <row r="118" spans="1:11">
       <c r="A118" s="17" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B118" s="18" t="s">
         <v>446</v>
@@ -6806,7 +6829,7 @@
         <v>508</v>
       </c>
       <c r="F118" s="15" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="G118" s="15">
         <v>1999</v>
@@ -6824,38 +6847,38 @@
     </row>
     <row r="119" spans="1:11">
       <c r="A119" s="17" t="s">
-        <v>192</v>
+        <v>171</v>
       </c>
       <c r="B119" s="18" t="s">
         <v>446</v>
       </c>
-      <c r="C119" s="15" t="s">
-        <v>462</v>
+      <c r="C119" s="17" t="s">
+        <v>468</v>
       </c>
       <c r="D119" s="15"/>
-      <c r="E119" s="15" t="s">
-        <v>509</v>
+      <c r="E119" s="17" t="s">
+        <v>508</v>
       </c>
       <c r="F119" s="15" t="s">
-        <v>282</v>
+        <v>262</v>
       </c>
       <c r="G119" s="15">
-        <v>1988</v>
+        <v>1999</v>
       </c>
       <c r="H119" s="15" t="s">
-        <v>440</v>
+        <v>66</v>
       </c>
       <c r="I119" s="16" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="J119" s="16" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="K119" s="16"/>
     </row>
     <row r="120" spans="1:11">
       <c r="A120" s="17" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B120" s="18" t="s">
         <v>446</v>
@@ -6868,7 +6891,7 @@
         <v>509</v>
       </c>
       <c r="F120" s="15" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G120" s="15">
         <v>1988</v>
@@ -6886,7 +6909,7 @@
     </row>
     <row r="121" spans="1:11">
       <c r="A121" s="17" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B121" s="18" t="s">
         <v>446</v>
@@ -6899,13 +6922,13 @@
         <v>509</v>
       </c>
       <c r="F121" s="15" t="s">
-        <v>284</v>
-      </c>
-      <c r="G121" s="15" t="s">
-        <v>14</v>
+        <v>283</v>
+      </c>
+      <c r="G121" s="15">
+        <v>1988</v>
       </c>
       <c r="H121" s="15" t="s">
-        <v>33</v>
+        <v>440</v>
       </c>
       <c r="I121" s="16" t="s">
         <v>418</v>
@@ -6917,38 +6940,38 @@
     </row>
     <row r="122" spans="1:11">
       <c r="A122" s="17" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="B122" s="18" t="s">
         <v>446</v>
       </c>
-      <c r="C122" s="17" t="s">
-        <v>463</v>
+      <c r="C122" s="15" t="s">
+        <v>462</v>
       </c>
       <c r="D122" s="15"/>
-      <c r="E122" s="17" t="s">
-        <v>510</v>
+      <c r="E122" s="15" t="s">
+        <v>509</v>
       </c>
       <c r="F122" s="15" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="G122" s="15" t="s">
         <v>14</v>
       </c>
       <c r="H122" s="15" t="s">
-        <v>441</v>
+        <v>33</v>
       </c>
       <c r="I122" s="16" t="s">
-        <v>363</v>
+        <v>418</v>
       </c>
       <c r="J122" s="16" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="K122" s="16"/>
     </row>
     <row r="123" spans="1:11">
       <c r="A123" s="17" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="B123" s="18" t="s">
         <v>446</v>
@@ -6960,8 +6983,8 @@
       <c r="E123" s="17" t="s">
         <v>510</v>
       </c>
-      <c r="F123" s="15">
-        <v>239</v>
+      <c r="F123" s="15" t="s">
+        <v>289</v>
       </c>
       <c r="G123" s="15" t="s">
         <v>14</v>
@@ -6970,47 +6993,47 @@
         <v>441</v>
       </c>
       <c r="I123" s="16" t="s">
-        <v>419</v>
+        <v>363</v>
       </c>
       <c r="J123" s="16" t="s">
-        <v>399</v>
+        <v>402</v>
       </c>
       <c r="K123" s="16"/>
     </row>
     <row r="124" spans="1:11">
       <c r="A124" s="17" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B124" s="18" t="s">
         <v>446</v>
       </c>
       <c r="C124" s="17" t="s">
-        <v>458</v>
+        <v>463</v>
       </c>
       <c r="D124" s="15"/>
       <c r="E124" s="17" t="s">
-        <v>511</v>
-      </c>
-      <c r="F124" s="15" t="s">
-        <v>286</v>
+        <v>510</v>
+      </c>
+      <c r="F124" s="15">
+        <v>239</v>
       </c>
       <c r="G124" s="15" t="s">
         <v>14</v>
       </c>
       <c r="H124" s="15" t="s">
-        <v>361</v>
+        <v>441</v>
       </c>
       <c r="I124" s="16" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="J124" s="16" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="K124" s="16"/>
     </row>
     <row r="125" spans="1:11">
       <c r="A125" s="17" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B125" s="18" t="s">
         <v>446</v>
@@ -7023,13 +7046,13 @@
         <v>511</v>
       </c>
       <c r="F125" s="15" t="s">
-        <v>287</v>
-      </c>
-      <c r="G125" s="15">
-        <v>1998</v>
+        <v>286</v>
+      </c>
+      <c r="G125" s="15" t="s">
+        <v>14</v>
       </c>
       <c r="H125" s="15" t="s">
-        <v>66</v>
+        <v>361</v>
       </c>
       <c r="I125" s="16" t="s">
         <v>421</v>
@@ -7041,7 +7064,7 @@
     </row>
     <row r="126" spans="1:11">
       <c r="A126" s="17" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B126" s="18" t="s">
         <v>446</v>
@@ -7054,13 +7077,13 @@
         <v>511</v>
       </c>
       <c r="F126" s="15" t="s">
-        <v>288</v>
-      </c>
-      <c r="G126" s="15" t="s">
-        <v>14</v>
+        <v>287</v>
+      </c>
+      <c r="G126" s="15">
+        <v>1998</v>
       </c>
       <c r="H126" s="15" t="s">
-        <v>361</v>
+        <v>66</v>
       </c>
       <c r="I126" s="16" t="s">
         <v>421</v>
@@ -7072,7 +7095,7 @@
     </row>
     <row r="127" spans="1:11">
       <c r="A127" s="17" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B127" s="18" t="s">
         <v>446</v>
@@ -7084,14 +7107,14 @@
       <c r="E127" s="17" t="s">
         <v>511</v>
       </c>
-      <c r="F127" s="15">
-        <v>5440</v>
+      <c r="F127" s="15" t="s">
+        <v>288</v>
       </c>
       <c r="G127" s="15" t="s">
         <v>14</v>
       </c>
       <c r="H127" s="15" t="s">
-        <v>14</v>
+        <v>361</v>
       </c>
       <c r="I127" s="16" t="s">
         <v>421</v>
@@ -7103,38 +7126,38 @@
     </row>
     <row r="128" spans="1:11">
       <c r="A128" s="17" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B128" s="18" t="s">
         <v>446</v>
       </c>
       <c r="C128" s="17" t="s">
-        <v>471</v>
+        <v>458</v>
       </c>
       <c r="D128" s="15"/>
       <c r="E128" s="17" t="s">
-        <v>512</v>
-      </c>
-      <c r="F128" s="15" t="s">
-        <v>291</v>
-      </c>
-      <c r="G128" s="15">
-        <v>2001</v>
+        <v>511</v>
+      </c>
+      <c r="F128" s="15">
+        <v>5440</v>
+      </c>
+      <c r="G128" s="15" t="s">
+        <v>14</v>
       </c>
       <c r="H128" s="15" t="s">
-        <v>66</v>
+        <v>14</v>
       </c>
       <c r="I128" s="16" t="s">
-        <v>372</v>
+        <v>421</v>
       </c>
       <c r="J128" s="16" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="K128" s="16"/>
     </row>
     <row r="129" spans="1:11">
       <c r="A129" s="17" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B129" s="18" t="s">
         <v>446</v>
@@ -7147,7 +7170,7 @@
         <v>512</v>
       </c>
       <c r="F129" s="15" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="G129" s="15">
         <v>2001</v>
@@ -7165,7 +7188,7 @@
     </row>
     <row r="130" spans="1:11">
       <c r="A130" s="17" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B130" s="18" t="s">
         <v>446</v>
@@ -7178,13 +7201,13 @@
         <v>512</v>
       </c>
       <c r="F130" s="15" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="G130" s="15">
-        <v>2009</v>
+        <v>2001</v>
       </c>
       <c r="H130" s="15" t="s">
-        <v>361</v>
+        <v>66</v>
       </c>
       <c r="I130" s="16" t="s">
         <v>372</v>
@@ -7196,69 +7219,69 @@
     </row>
     <row r="131" spans="1:11">
       <c r="A131" s="17" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B131" s="18" t="s">
         <v>446</v>
       </c>
       <c r="C131" s="17" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="D131" s="15"/>
       <c r="E131" s="17" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="F131" s="15" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="G131" s="15">
-        <v>1997</v>
+        <v>2009</v>
       </c>
       <c r="H131" s="15" t="s">
-        <v>442</v>
+        <v>361</v>
       </c>
       <c r="I131" s="16" t="s">
-        <v>364</v>
+        <v>372</v>
       </c>
       <c r="J131" s="16" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="K131" s="16"/>
     </row>
     <row r="132" spans="1:11">
       <c r="A132" s="17" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B132" s="18" t="s">
         <v>446</v>
       </c>
       <c r="C132" s="17" t="s">
-        <v>457</v>
+        <v>472</v>
       </c>
       <c r="D132" s="15"/>
       <c r="E132" s="17" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="F132" s="15" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G132" s="15">
-        <v>2000</v>
+        <v>1997</v>
       </c>
       <c r="H132" s="15" t="s">
-        <v>66</v>
+        <v>442</v>
       </c>
       <c r="I132" s="16" t="s">
-        <v>371</v>
+        <v>364</v>
       </c>
       <c r="J132" s="16" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="K132" s="16"/>
     </row>
     <row r="133" spans="1:11">
       <c r="A133" s="17" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B133" s="18" t="s">
         <v>446</v>
@@ -7271,10 +7294,10 @@
         <v>514</v>
       </c>
       <c r="F133" s="15" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="G133" s="15">
-        <v>2002</v>
+        <v>2000</v>
       </c>
       <c r="H133" s="15" t="s">
         <v>66</v>
@@ -7289,7 +7312,7 @@
     </row>
     <row r="134" spans="1:11">
       <c r="A134" s="17" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B134" s="18" t="s">
         <v>446</v>
@@ -7302,13 +7325,13 @@
         <v>514</v>
       </c>
       <c r="F134" s="15" t="s">
-        <v>297</v>
-      </c>
-      <c r="G134" s="15" t="s">
-        <v>14</v>
+        <v>296</v>
+      </c>
+      <c r="G134" s="15">
+        <v>2002</v>
       </c>
       <c r="H134" s="15" t="s">
-        <v>361</v>
+        <v>66</v>
       </c>
       <c r="I134" s="16" t="s">
         <v>371</v>
@@ -7320,7 +7343,7 @@
     </row>
     <row r="135" spans="1:11">
       <c r="A135" s="17" t="s">
-        <v>359</v>
+        <v>209</v>
       </c>
       <c r="B135" s="18" t="s">
         <v>446</v>
@@ -7332,11 +7355,15 @@
       <c r="E135" s="17" t="s">
         <v>514</v>
       </c>
-      <c r="F135" s="16" t="s">
-        <v>360</v>
-      </c>
-      <c r="G135" s="15"/>
-      <c r="H135" s="16"/>
+      <c r="F135" s="15" t="s">
+        <v>297</v>
+      </c>
+      <c r="G135" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="H135" s="15" t="s">
+        <v>361</v>
+      </c>
       <c r="I135" s="16" t="s">
         <v>371</v>
       </c>
@@ -7347,38 +7374,34 @@
     </row>
     <row r="136" spans="1:11">
       <c r="A136" s="17" t="s">
-        <v>139</v>
+        <v>359</v>
       </c>
       <c r="B136" s="18" t="s">
         <v>446</v>
       </c>
       <c r="C136" s="17" t="s">
-        <v>467</v>
+        <v>457</v>
       </c>
       <c r="D136" s="15"/>
       <c r="E136" s="17" t="s">
-        <v>515</v>
-      </c>
-      <c r="F136" s="15" t="s">
-        <v>230</v>
-      </c>
-      <c r="G136" s="15">
-        <v>2013</v>
-      </c>
-      <c r="H136" s="15" t="s">
-        <v>440</v>
-      </c>
+        <v>514</v>
+      </c>
+      <c r="F136" s="16" t="s">
+        <v>360</v>
+      </c>
+      <c r="G136" s="15"/>
+      <c r="H136" s="16"/>
       <c r="I136" s="16" t="s">
-        <v>411</v>
+        <v>371</v>
       </c>
       <c r="J136" s="16" t="s">
-        <v>392</v>
+        <v>405</v>
       </c>
       <c r="K136" s="16"/>
     </row>
     <row r="137" spans="1:11">
       <c r="A137" s="17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B137" s="18" t="s">
         <v>446</v>
@@ -7391,13 +7414,13 @@
         <v>515</v>
       </c>
       <c r="F137" s="15" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G137" s="15">
-        <v>2010</v>
+        <v>2013</v>
       </c>
       <c r="H137" s="15" t="s">
-        <v>30</v>
+        <v>440</v>
       </c>
       <c r="I137" s="16" t="s">
         <v>411</v>
@@ -7409,7 +7432,7 @@
     </row>
     <row r="138" spans="1:11">
       <c r="A138" s="17" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B138" s="18" t="s">
         <v>446</v>
@@ -7422,7 +7445,7 @@
         <v>515</v>
       </c>
       <c r="F138" s="15" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G138" s="15">
         <v>2010</v>
@@ -7440,7 +7463,7 @@
     </row>
     <row r="139" spans="1:11">
       <c r="A139" s="17" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B139" s="18" t="s">
         <v>446</v>
@@ -7453,7 +7476,7 @@
         <v>515</v>
       </c>
       <c r="F139" s="15" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G139" s="15">
         <v>2010</v>
@@ -7471,69 +7494,69 @@
     </row>
     <row r="140" spans="1:11">
       <c r="A140" s="17" t="s">
-        <v>210</v>
+        <v>142</v>
       </c>
       <c r="B140" s="18" t="s">
         <v>446</v>
       </c>
       <c r="C140" s="17" t="s">
-        <v>460</v>
+        <v>467</v>
       </c>
       <c r="D140" s="15"/>
       <c r="E140" s="17" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="F140" s="15" t="s">
-        <v>298</v>
-      </c>
-      <c r="G140" s="15" t="s">
-        <v>14</v>
+        <v>233</v>
+      </c>
+      <c r="G140" s="15">
+        <v>2010</v>
       </c>
       <c r="H140" s="15" t="s">
-        <v>317</v>
+        <v>30</v>
       </c>
       <c r="I140" s="16" t="s">
-        <v>370</v>
+        <v>411</v>
       </c>
       <c r="J140" s="16" t="s">
-        <v>403</v>
+        <v>392</v>
       </c>
       <c r="K140" s="16"/>
     </row>
     <row r="141" spans="1:11">
       <c r="A141" s="17" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B141" s="18" t="s">
         <v>446</v>
       </c>
       <c r="C141" s="17" t="s">
-        <v>347</v>
+        <v>460</v>
       </c>
       <c r="D141" s="15"/>
       <c r="E141" s="17" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="F141" s="15" t="s">
-        <v>299</v>
-      </c>
-      <c r="G141" s="15">
-        <v>1979</v>
+        <v>298</v>
+      </c>
+      <c r="G141" s="15" t="s">
+        <v>14</v>
       </c>
       <c r="H141" s="15" t="s">
-        <v>442</v>
-      </c>
-      <c r="I141" s="15" t="s">
-        <v>427</v>
+        <v>317</v>
+      </c>
+      <c r="I141" s="16" t="s">
+        <v>370</v>
       </c>
       <c r="J141" s="16" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="K141" s="16"/>
     </row>
     <row r="142" spans="1:11">
       <c r="A142" s="17" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B142" s="18" t="s">
         <v>446</v>
@@ -7546,13 +7569,13 @@
         <v>517</v>
       </c>
       <c r="F142" s="15" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="G142" s="15">
-        <v>1992</v>
+        <v>1979</v>
       </c>
       <c r="H142" s="15" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="I142" s="15" t="s">
         <v>427</v>
@@ -7564,7 +7587,7 @@
     </row>
     <row r="143" spans="1:11">
       <c r="A143" s="17" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B143" s="18" t="s">
         <v>446</v>
@@ -7577,7 +7600,7 @@
         <v>517</v>
       </c>
       <c r="F143" s="15" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="G143" s="15">
         <v>1992</v>
@@ -7595,7 +7618,7 @@
     </row>
     <row r="144" spans="1:11">
       <c r="A144" s="17" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B144" s="18" t="s">
         <v>446</v>
@@ -7608,13 +7631,13 @@
         <v>517</v>
       </c>
       <c r="F144" s="15" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="G144" s="15">
-        <v>2006</v>
+        <v>1992</v>
       </c>
       <c r="H144" s="15" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="I144" s="15" t="s">
         <v>427</v>
@@ -7626,7 +7649,7 @@
     </row>
     <row r="145" spans="1:11">
       <c r="A145" s="17" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B145" s="18" t="s">
         <v>446</v>
@@ -7639,10 +7662,10 @@
         <v>517</v>
       </c>
       <c r="F145" s="15" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="G145" s="15">
-        <v>2011</v>
+        <v>2006</v>
       </c>
       <c r="H145" s="15" t="s">
         <v>441</v>
@@ -7657,7 +7680,7 @@
     </row>
     <row r="146" spans="1:11">
       <c r="A146" s="17" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B146" s="18" t="s">
         <v>446</v>
@@ -7670,10 +7693,10 @@
         <v>517</v>
       </c>
       <c r="F146" s="15" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G146" s="15">
-        <v>1986</v>
+        <v>2011</v>
       </c>
       <c r="H146" s="15" t="s">
         <v>441</v>
@@ -7688,7 +7711,7 @@
     </row>
     <row r="147" spans="1:11">
       <c r="A147" s="17" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B147" s="18" t="s">
         <v>446</v>
@@ -7701,10 +7724,10 @@
         <v>517</v>
       </c>
       <c r="F147" s="15" t="s">
-        <v>305</v>
-      </c>
-      <c r="G147" s="15" t="s">
-        <v>14</v>
+        <v>304</v>
+      </c>
+      <c r="G147" s="15">
+        <v>1986</v>
       </c>
       <c r="H147" s="15" t="s">
         <v>441</v>
@@ -7719,7 +7742,7 @@
     </row>
     <row r="148" spans="1:11">
       <c r="A148" s="17" t="s">
-        <v>346</v>
+        <v>217</v>
       </c>
       <c r="B148" s="18" t="s">
         <v>446</v>
@@ -7731,12 +7754,16 @@
       <c r="E148" s="17" t="s">
         <v>517</v>
       </c>
-      <c r="F148" s="16" t="s">
-        <v>347</v>
-      </c>
-      <c r="G148" s="15"/>
-      <c r="H148" s="16"/>
-      <c r="I148" s="16" t="s">
+      <c r="F148" s="15" t="s">
+        <v>305</v>
+      </c>
+      <c r="G148" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="H148" s="15" t="s">
+        <v>441</v>
+      </c>
+      <c r="I148" s="15" t="s">
         <v>427</v>
       </c>
       <c r="J148" s="16" t="s">
@@ -7746,69 +7773,65 @@
     </row>
     <row r="149" spans="1:11">
       <c r="A149" s="17" t="s">
-        <v>218</v>
+        <v>346</v>
       </c>
       <c r="B149" s="18" t="s">
         <v>446</v>
       </c>
       <c r="C149" s="17" t="s">
-        <v>473</v>
+        <v>347</v>
       </c>
       <c r="D149" s="15"/>
       <c r="E149" s="17" t="s">
-        <v>518</v>
-      </c>
-      <c r="F149" s="15" t="s">
-        <v>306</v>
-      </c>
-      <c r="G149" s="15">
-        <v>1998</v>
-      </c>
-      <c r="H149" s="15" t="s">
-        <v>361</v>
-      </c>
+        <v>517</v>
+      </c>
+      <c r="F149" s="16" t="s">
+        <v>347</v>
+      </c>
+      <c r="G149" s="15"/>
+      <c r="H149" s="16"/>
       <c r="I149" s="16" t="s">
-        <v>365</v>
+        <v>427</v>
       </c>
       <c r="J149" s="16" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="K149" s="16"/>
     </row>
     <row r="150" spans="1:11">
       <c r="A150" s="17" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B150" s="18" t="s">
         <v>446</v>
       </c>
       <c r="C150" s="17" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="D150" s="15"/>
       <c r="E150" s="17" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="F150" s="15" t="s">
-        <v>307</v>
-      </c>
-      <c r="G150" s="15" t="s">
-        <v>14</v>
+        <v>306</v>
+      </c>
+      <c r="G150" s="15">
+        <v>1998</v>
       </c>
       <c r="H150" s="15" t="s">
-        <v>33</v>
+        <v>361</v>
       </c>
       <c r="I150" s="16" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="J150" s="16" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="K150" s="16"/>
     </row>
     <row r="151" spans="1:11">
       <c r="A151" s="17" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B151" s="18" t="s">
         <v>446</v>
@@ -7821,7 +7844,7 @@
         <v>519</v>
       </c>
       <c r="F151" s="15" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G151" s="15" t="s">
         <v>14</v>
@@ -7839,38 +7862,38 @@
     </row>
     <row r="152" spans="1:11">
       <c r="A152" s="17" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B152" s="18" t="s">
         <v>446</v>
       </c>
       <c r="C152" s="17" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="D152" s="15"/>
       <c r="E152" s="17" t="s">
-        <v>520</v>
-      </c>
-      <c r="F152" s="15">
-        <v>266</v>
-      </c>
-      <c r="G152" s="15">
-        <v>2000</v>
+        <v>519</v>
+      </c>
+      <c r="F152" s="15" t="s">
+        <v>308</v>
+      </c>
+      <c r="G152" s="15" t="s">
+        <v>14</v>
       </c>
       <c r="H152" s="15" t="s">
-        <v>66</v>
+        <v>33</v>
       </c>
       <c r="I152" s="16" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="J152" s="16" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="K152" s="16"/>
     </row>
     <row r="153" spans="1:11">
       <c r="A153" s="17" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B153" s="18" t="s">
         <v>446</v>
@@ -7883,10 +7906,10 @@
         <v>520</v>
       </c>
       <c r="F153" s="15">
-        <v>8023</v>
+        <v>266</v>
       </c>
       <c r="G153" s="15">
-        <v>2001</v>
+        <v>2000</v>
       </c>
       <c r="H153" s="15" t="s">
         <v>66</v>
@@ -7901,38 +7924,38 @@
     </row>
     <row r="154" spans="1:11">
       <c r="A154" s="17" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="B154" s="18" t="s">
         <v>446</v>
       </c>
       <c r="C154" s="17" t="s">
-        <v>466</v>
+        <v>475</v>
       </c>
       <c r="D154" s="15"/>
       <c r="E154" s="17" t="s">
-        <v>521</v>
-      </c>
-      <c r="F154" s="15" t="s">
-        <v>314</v>
+        <v>520</v>
+      </c>
+      <c r="F154" s="15">
+        <v>8023</v>
       </c>
       <c r="G154" s="15">
-        <v>1998</v>
+        <v>2001</v>
       </c>
       <c r="H154" s="15" t="s">
-        <v>442</v>
+        <v>66</v>
       </c>
       <c r="I154" s="16" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="J154" s="16" t="s">
-        <v>426</v>
+        <v>410</v>
       </c>
       <c r="K154" s="16"/>
     </row>
     <row r="155" spans="1:11">
       <c r="A155" s="17" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B155" s="18" t="s">
         <v>446</v>
@@ -7945,13 +7968,13 @@
         <v>521</v>
       </c>
       <c r="F155" s="15" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="G155" s="15">
-        <v>2005</v>
+        <v>1998</v>
       </c>
       <c r="H155" s="15" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="I155" s="16" t="s">
         <v>369</v>
@@ -7963,170 +7986,201 @@
     </row>
     <row r="156" spans="1:11">
       <c r="A156" s="17" t="s">
-        <v>477</v>
+        <v>229</v>
       </c>
       <c r="B156" s="18" t="s">
         <v>446</v>
       </c>
       <c r="C156" s="17" t="s">
-        <v>462</v>
+        <v>466</v>
       </c>
       <c r="D156" s="15"/>
       <c r="E156" s="17" t="s">
-        <v>509</v>
-      </c>
-      <c r="F156" s="16" t="s">
-        <v>478</v>
-      </c>
-      <c r="G156" s="16"/>
-      <c r="H156" s="16"/>
+        <v>521</v>
+      </c>
+      <c r="F156" s="15" t="s">
+        <v>315</v>
+      </c>
+      <c r="G156" s="15">
+        <v>2005</v>
+      </c>
+      <c r="H156" s="15" t="s">
+        <v>444</v>
+      </c>
       <c r="I156" s="16" t="s">
-        <v>418</v>
+        <v>369</v>
       </c>
       <c r="J156" s="16" t="s">
-        <v>398</v>
-      </c>
-      <c r="K156" s="9"/>
+        <v>426</v>
+      </c>
+      <c r="K156" s="16"/>
     </row>
     <row r="157" spans="1:11">
       <c r="A157" s="17" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="B157" s="18" t="s">
         <v>446</v>
       </c>
       <c r="C157" s="17" t="s">
-        <v>479</v>
+        <v>462</v>
       </c>
       <c r="D157" s="15"/>
       <c r="E157" s="17" t="s">
-        <v>522</v>
+        <v>509</v>
       </c>
       <c r="F157" s="16" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="G157" s="16"/>
       <c r="H157" s="16"/>
       <c r="I157" s="16" t="s">
-        <v>375</v>
+        <v>418</v>
       </c>
       <c r="J157" s="16" t="s">
-        <v>425</v>
+        <v>398</v>
       </c>
       <c r="K157" s="9"/>
     </row>
     <row r="158" spans="1:11">
       <c r="A158" s="17" t="s">
-        <v>332</v>
+        <v>476</v>
       </c>
       <c r="B158" s="18" t="s">
-        <v>487</v>
+        <v>446</v>
       </c>
       <c r="C158" s="17" t="s">
-        <v>383</v>
+        <v>479</v>
       </c>
       <c r="D158" s="15"/>
-      <c r="F158" t="s">
-        <v>333</v>
-      </c>
-      <c r="I158" t="s">
-        <v>481</v>
+      <c r="E158" s="17" t="s">
+        <v>522</v>
+      </c>
+      <c r="F158" s="16" t="s">
+        <v>479</v>
+      </c>
+      <c r="G158" s="16"/>
+      <c r="H158" s="16"/>
+      <c r="I158" s="16" t="s">
+        <v>375</v>
+      </c>
+      <c r="J158" s="16" t="s">
+        <v>425</v>
       </c>
       <c r="K158" s="9"/>
     </row>
     <row r="159" spans="1:11">
       <c r="A159" s="17" t="s">
-        <v>344</v>
+        <v>332</v>
       </c>
       <c r="B159" s="18" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="C159" s="17" t="s">
-        <v>343</v>
-      </c>
-      <c r="D159" s="15" t="s">
-        <v>454</v>
-      </c>
-      <c r="E159" s="16"/>
+        <v>383</v>
+      </c>
+      <c r="D159" s="15"/>
       <c r="F159" t="s">
-        <v>486</v>
-      </c>
-      <c r="H159" t="s">
-        <v>485</v>
-      </c>
-      <c r="I159" s="16" t="s">
-        <v>496</v>
-      </c>
-      <c r="J159" s="16" t="s">
-        <v>484</v>
+        <v>333</v>
+      </c>
+      <c r="I159" t="s">
+        <v>481</v>
       </c>
       <c r="K159" s="9"/>
     </row>
     <row r="160" spans="1:11">
       <c r="A160" s="17" t="s">
+        <v>344</v>
+      </c>
+      <c r="B160" s="18" t="s">
+        <v>488</v>
+      </c>
+      <c r="C160" s="17" t="s">
+        <v>343</v>
+      </c>
+      <c r="D160" s="15" t="s">
+        <v>454</v>
+      </c>
+      <c r="E160" s="16"/>
+      <c r="F160" t="s">
+        <v>486</v>
+      </c>
+      <c r="H160" t="s">
+        <v>485</v>
+      </c>
+      <c r="I160" s="16" t="s">
+        <v>496</v>
+      </c>
+      <c r="J160" s="16" t="s">
+        <v>484</v>
+      </c>
+      <c r="K160" s="9"/>
+    </row>
+    <row r="161" spans="1:11">
+      <c r="A161" s="17" t="s">
         <v>338</v>
       </c>
-      <c r="B160" s="18" t="s">
+      <c r="B161" s="18" t="s">
         <v>489</v>
-      </c>
-      <c r="C160" s="18"/>
-      <c r="D160" s="15"/>
-      <c r="F160" t="s">
-        <v>482</v>
-      </c>
-      <c r="I160" s="16" t="s">
-        <v>495</v>
-      </c>
-      <c r="J160" s="16" t="s">
-        <v>483</v>
-      </c>
-      <c r="K160" s="9"/>
-    </row>
-    <row r="161" spans="1:10">
-      <c r="A161" s="17" t="s">
-        <v>330</v>
-      </c>
-      <c r="B161" s="18" t="s">
-        <v>487</v>
       </c>
       <c r="C161" s="18"/>
       <c r="D161" s="15"/>
-      <c r="F161" s="35" t="s">
+      <c r="F161" t="s">
+        <v>482</v>
+      </c>
+      <c r="I161" s="16" t="s">
+        <v>495</v>
+      </c>
+      <c r="J161" s="16" t="s">
+        <v>483</v>
+      </c>
+      <c r="K161" s="9"/>
+    </row>
+    <row r="162" spans="1:11">
+      <c r="A162" s="17" t="s">
+        <v>330</v>
+      </c>
+      <c r="B162" s="18" t="s">
+        <v>487</v>
+      </c>
+      <c r="C162" s="18"/>
+      <c r="D162" s="15"/>
+      <c r="F162" s="35" t="s">
         <v>492</v>
-      </c>
-      <c r="H161" t="s">
-        <v>19</v>
-      </c>
-      <c r="I161" s="16" t="s">
-        <v>497</v>
-      </c>
-      <c r="J161" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="162" spans="1:10">
-      <c r="A162" s="17" t="s">
-        <v>384</v>
-      </c>
-      <c r="B162" s="18" t="s">
-        <v>488</v>
-      </c>
-      <c r="C162" s="17" t="s">
-        <v>345</v>
-      </c>
-      <c r="D162" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="F162" s="35" t="s">
-        <v>490</v>
       </c>
       <c r="H162" t="s">
         <v>19</v>
       </c>
       <c r="I162" s="16" t="s">
+        <v>497</v>
+      </c>
+      <c r="J162" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="163" spans="1:11">
+      <c r="A163" s="17" t="s">
+        <v>384</v>
+      </c>
+      <c r="B163" s="18" t="s">
+        <v>488</v>
+      </c>
+      <c r="C163" s="17" t="s">
+        <v>345</v>
+      </c>
+      <c r="D163" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="F163" s="35" t="s">
+        <v>490</v>
+      </c>
+      <c r="H163" t="s">
+        <v>19</v>
+      </c>
+      <c r="I163" s="16" t="s">
         <v>494</v>
       </c>
-      <c r="J162" s="16" t="s">
+      <c r="J163" s="16" t="s">
         <v>491</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Incorporated PLV alignment derived from Los Alamos database
</commit_message>
<xml_diff>
--- a/tabular/hiv-reference-data.xlsx
+++ b/tabular/hiv-reference-data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10917"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/Ortervirales/HIV-GLUE/tabular/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AECDEBD-7886-1444-9016-727559567D5B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C93BFD7-AC5A-0944-9A8F-EC9E59CF75D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9640" yWindow="460" windowWidth="25460" windowHeight="25220" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2553" uniqueCount="526">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2574" uniqueCount="535">
   <si>
     <t>Accession</t>
   </si>
@@ -1605,13 +1605,40 @@
   </si>
   <si>
     <t>Ferret</t>
+  </si>
+  <si>
+    <t>AY618998</t>
+  </si>
+  <si>
+    <t>JN091691</t>
+  </si>
+  <si>
+    <t>M76764</t>
+  </si>
+  <si>
+    <t>M19499</t>
+  </si>
+  <si>
+    <t>JQ864084</t>
+  </si>
+  <si>
+    <t>JX648292</t>
+  </si>
+  <si>
+    <t>JX648291</t>
+  </si>
+  <si>
+    <t>MF370842</t>
+  </si>
+  <si>
+    <t>SIVtan</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1666,6 +1693,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="12">
@@ -2147,7 +2180,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2224,6 +2257,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="376">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2603,15 +2637,7 @@
     <cellStyle name="Hyperlink" xfId="374" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD9D9D9"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -2955,10 +2981,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S162"/>
+  <dimension ref="A1:S170"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="A131" workbookViewId="0">
+      <selection activeCell="C166" sqref="C166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8156,9 +8182,88 @@
         <v>491</v>
       </c>
     </row>
+    <row r="163" spans="1:10" ht="17" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>526</v>
+      </c>
+      <c r="B163" s="18" t="s">
+        <v>446</v>
+      </c>
+      <c r="C163" s="36" t="s">
+        <v>348</v>
+      </c>
+      <c r="D163" s="36" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="164" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A164" t="s">
+        <v>527</v>
+      </c>
+      <c r="B164" s="18" t="s">
+        <v>446</v>
+      </c>
+      <c r="C164" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="165" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A165" t="s">
+        <v>528</v>
+      </c>
+      <c r="B165" s="18" t="s">
+        <v>446</v>
+      </c>
+      <c r="C165" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="166" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A166" t="s">
+        <v>529</v>
+      </c>
+      <c r="B166" s="18" t="s">
+        <v>446</v>
+      </c>
+      <c r="C166" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="167" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A167" t="s">
+        <v>530</v>
+      </c>
+      <c r="B167" s="18" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="168" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A168" t="s">
+        <v>531</v>
+      </c>
+      <c r="B168" s="18" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="169" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A169" t="s">
+        <v>532</v>
+      </c>
+      <c r="B169" s="18" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="170" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A170" t="s">
+        <v>533</v>
+      </c>
+      <c r="B170" s="18" t="s">
+        <v>446</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L151">
-    <sortCondition sortBy="cellColor" ref="C2:C151" dxfId="1"/>
+    <sortCondition sortBy="cellColor" ref="C2:C151" dxfId="0"/>
     <sortCondition ref="C2:C151"/>
     <sortCondition ref="D2:D151"/>
     <sortCondition ref="E2:E151"/>

</xml_diff>

<commit_message>
Updated reference sequence side data with new taxa
</commit_message>
<xml_diff>
--- a/tabular/hiv-reference-data.xlsx
+++ b/tabular/hiv-reference-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/Ortervirales/HIV-GLUE/tabular/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C93BFD7-AC5A-0944-9A8F-EC9E59CF75D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B560EDE-D00E-DD40-A900-367390E3D38D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9640" yWindow="460" windowWidth="25460" windowHeight="25220" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23620" yWindow="460" windowWidth="25460" windowHeight="25220" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="edited down" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2574" uniqueCount="535">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2578" uniqueCount="536">
   <si>
     <t>Accession</t>
   </si>
@@ -1632,6 +1632,9 @@
   </si>
   <si>
     <t>SIVtan</t>
+  </si>
+  <si>
+    <t>SIVsm</t>
   </si>
 </sst>
 </file>
@@ -2983,8 +2986,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S170"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A131" workbookViewId="0">
-      <selection activeCell="C166" sqref="C166"/>
+    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="B169" sqref="A1:K170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8236,6 +8239,9 @@
       <c r="B167" s="18" t="s">
         <v>446</v>
       </c>
+      <c r="C167" t="s">
+        <v>535</v>
+      </c>
     </row>
     <row r="168" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
@@ -8244,6 +8250,9 @@
       <c r="B168" s="18" t="s">
         <v>446</v>
       </c>
+      <c r="C168" t="s">
+        <v>463</v>
+      </c>
     </row>
     <row r="169" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
@@ -8252,6 +8261,9 @@
       <c r="B169" s="18" t="s">
         <v>446</v>
       </c>
+      <c r="C169" t="s">
+        <v>535</v>
+      </c>
     </row>
     <row r="170" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
@@ -8259,6 +8271,9 @@
       </c>
       <c r="B170" s="18" t="s">
         <v>446</v>
+      </c>
+      <c r="C170" t="s">
+        <v>535</v>
       </c>
     </row>
   </sheetData>

</xml_diff>